<commit_message>
More info for RAG
</commit_message>
<xml_diff>
--- a/data/Info RAG.xlsx
+++ b/data/Info RAG.xlsx
@@ -7,14 +7,14 @@
     <sheet state="visible" name="Info RAG" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Info RAG'!$C$1:$C$1000</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Info RAG'!$C$1:$C$992</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="168">
   <si>
     <t>Problemas abordados</t>
   </si>
@@ -602,9 +602,941 @@
     <t>https://www.medley.com.br/saude-e-bem-estar/saude-fisica/cuidados/destaques/efeito-pratica-esporte-depressao</t>
   </si>
   <si>
-    <t xml:space="preserve">ATIVIDADE FÍSICA:
+    <t>ALIMENTOS PARA AJUDAR NA CICATRIZAÇÃO / INFLAMAÇÕES
 INDICAÇÕES:
+1. Proteínas
+As proteínas são fundamentais para os tecidos dos tecidos e a cicatrização de feridas. Eles fornecem os blocos de construção necessários para a descrição de novas células e tecidos, essenciais para o fechamento e a recuperação das lesões cirúrgicas.
+Carnes magras: Frango, Peru e cortes magros de carne bovina fornecem proteínas de alta qualidade que são rapidamente absorvidas pelo corpo.
+Peixes: Principalmente os ricos em ômega-3, como salmão e sardinha, que possuem propriedades anti-inflamatórias.
+Ovos: Uma excelente fonte de proteína completa e outros nutrientes componentes.
+Laticínios : Leite, iogurte e queijo ajudam na manutenção da massa muscular.
+Leguminosas: Feijões, lentilhas e grão-de-bico são fontes vegetais ricas em proteínas.
+Oleaginosas e sementes : Amêndoas, nozes e sementes de chia fornecem proteínas e gorduras saudáveis.
+2. Vitaminas e Minerais
+Vitamina C
+A vitamina C é crucial para a produção de colágeno, essencial para a cicatrização de feridas. Atua como antioxidante, protegendo as células do dano oxidativo.
+Frutas cítricas: Laranjas, limões e toranjas são ricas em vitamina C.
+Outras frutas: Morangos, kiwis e abacaxi com nutrientes para a riqueza do colágeno.
+Vegetais: Pimentões, brócolis e espinafre são ótimas fontes de vitamina C.
+Vitamina A
+A vitamina A é importante para a síntese do colágeno e para o funcionamento adequado do sistema imunológico.
+Vegetais laranja e amarelos: Cenouras, abóbora e batata-doce contêm altos níveis de betacaroteno, precursor da vitamina A.
+Vegetais verdes folhosos: Espinafre e couve fornecem vitamina A e outros antioxidantes.
+Zinco
+O zinco desempenha um papel vital na divisão celular e nas proteínas de proteínas, ambos necessários para a cicatrização.
+Carnes: Carne bovina, frango e cordeiro são fontes ricas em zinco.
+Frutos do mar: Ostras, caranguejos e lagostas têm altos níveis de zinco.
+Leguminosas: Feijões e lentilhas oferecem zinco em formas vegetais.
+Oleaginosas: Castanhas e sementes são boas fontes vegetais de zinco.
+Ferro
+O ferro é essencial para o transporte de oxigênio no sangue, crucial para a cicatrização de feridas.
+Carnes vermelhas: Fígado e carnes magras são ricas em ferro heme, facilmente absorvíveis.
+Vegetais verdes escuros: Espinafre e couve são boas fontes de ferro não-heme.
+Leguminosas: Feijões e lentilhas contêm ferro e fibras.
+Frutas secas: Damascos e passas são opções ricas em ferro.
+3. Ácidos Graxos Ômega-3
+Os ácidos graxos ômega-3 ajudam a reduzir a inflamação e podem melhorar o processo de cicatrização, atuando como anti-inflamatórios naturais.
+Peixes gordurosos : Salmão, sardinha e atum são ricos em ômega-3.
+Sementes de chia e linhaça : Fontes vegetais ricas em ômega-3.
+Nozes : Contêm ômega-3 e outras gorduras saudáveis.
+4. Hidratação
+Manter-se bem hidratado é essencial para a cicatrização de feridas, pois a água é necessária para quase todas as funções corporais, incluindo a manutenção do volume sanguíneo e a eliminação de toxinas.
+Água: Beba pelo menos 8 copos de água por dia para manter a hidratação.
+Chás de ervas: Sem adição de açúcar, ajuda na hidratação.
+Caldos claros: Sopas de frango ou vegetais são opções nutritivas e hidratantes.
+5. Antioxidantes
+Os antioxidantes ajudam a proteger as células dos danos causados ​​pelos radicais livres durante o processo inflamatório e a cicatrização
+.
+Frutas e vegetais coloridos: Frutas vermelhas, tomates e cenouras são ricos em antioxidantes.
+Chá verde: Rico em catequinas, antioxidantes potentes.
+Ervas e especiarias: Cúrcuma, gengibre e alho têm propriedades anti-inflamatórias e antioxidantes.
+CUIDADOS: Para maximizar os benefícios nutricionais, consulte um nutricionista para adaptar essas recomendações às suas necessidades específicas.</t>
+  </si>
+  <si>
+    <t>Alimentaç±ao saudável</t>
+  </si>
+  <si>
+    <t>https://www.posuscs.com.br/melhores-alimentos-para-ajudar-na-cicatrizacao-no-pos-operatorio/noticia/3099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR EM DISTÚRBIOS DIGESTIVOS
+A principal explicação para o surgimento de doenças do trato digestivo envolve o estilo de vida das pessoas. Isso inclui:
+– Sedentarismo;
+– Sono insuficiente (hábito muito associado ao uso de eletrônicos);
+– Tabagismo e alcoolismo;
+– Estresse excessivo;
+– Alimentação inadequada, como o consumo de fast food e uma dieta pobre em frutas e verduras.
+As enfermidades que mais acometem o aparelho digestivo são Doença do Refluxo Gastroesofágico, úlcera gástrica, gastrite, intolerância à lactose, apendicite, doenças inflamatórias intestinais. Infecções e maus hábitos alimentares são os principais fatores para o desenvolvimento de doenças e tumores na região.
+INDICAÇÕES:
+Mudanças de hábitos simples podem prevenir algumas delas. Gastrite e doença do refluxo podem ser prevenidas evitando a ingestão em excesso de condimentos, gorduras, frituras e de cafeína. Evitar ingerir líquidos enquanto come, melhorar a mastigação, fazer higiene adequada dos alimentos, não comer e deitar-se imediatamente, evitar excessos alimentares, principalmente à noite, são alguns hábitos que podem ajudar a melhorar a saúde digestiva.
+Alimentos que evitam ou aliviam os sintomas das doenças gastrointestinais:
+– Frutas, como mamão e abacaxi;
+– Água e chás;
+– Azeite;
+– Oleaginosas, como as castanhas e amêndoas;
+– Cereais integrais;
+– Massas à base de farinha de arroz;
+– Vegetais.
+Praticar uma dieta saudável, rica em fibra, é importante para manter o trânsito intestinal funcionando corretamente e evitar o surgimento das doenças gastrointestinais. Além disso, é necessário observar as reações do corpo ao ingerir qualquer alimento ou bebida, a fim de identificar o surgimento de sintomas e procurar um médico especialista.
+</t>
+  </si>
+  <si>
+    <t>https://bvsms.saude.gov.br/sua-saude-digestiva-nutrir-para-florescer-29-5-dia-mundial-da-saude-digestiva-2025/
+https://www.clinicacirurgicataguatinga.com.br/voce-sabia-que-a-ma-alimentacao-pode-agravar-as-doencas-gastrointestinais/</t>
+  </si>
+  <si>
+    <t>ALIMENTOS PARA AJUDAR A FADIGA
+INDICAÇÕES:
+Alguns dos principais alimentos que podem ajudar a combater o cansaço são:
+Maracujá;
+Abacate;
+Banana;
+Cereja;
+Alface;
+Canela;
+Chá de erva-cidreira;
+Mel;
+Amendoim;
+Ovos;
+Abóbora;
+Amêndoas;
+Espinafre;
+Aveia;
+Levedura de cerveja;
+Queijo;
+Cacau;
+Canela;
+Brócolis;
+Beterraba.
+Esses alimentos ajudam a estimular a produção de serotonina, que é um neurotransmissor relacionado com a sensação de prazer e bem-estar, e o relaxamento. Dessa forma, é possível combater o cansaço físico e o esgotamento mental.
+Esses alimentos devem ser consumidos 2 a 3 vezes por dia, por exemplo, alface na salada do almoço, banana com canela no lanche e suco de cereja antes de ir dormir.
+Outros alimentos, como café, chá verde ou guaraná ajudam a estimular o sistema nervoso central dando mais energia e, por isso, devem ser consumidos antes das 17 h para não causar insônia e prejudicar o descanso durante a noite.
+CUIDADOS: Se após uma ou duas semanas a fazer uma alimentação rica nesses alimentos o cansaço não diminuir, é aconselhado consultar um médico para verificar se existe algum problema de saúde.</t>
+  </si>
+  <si>
+    <t>https://www.tuasaude.com/alimentos-que-combatem-o-cansaco/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A DOR DE CABEÇA E ENXAQUECA
+Quem sofre com as crises de enxaqueca sabe o quanto isso é incômodo. Embora seja uma doença genética, crônica e afete 30 milhões de brasileiros há uma boa notícia: os sintomas podem ser amenizados com uma boa alimentação. Incluir na dieta alimentos como a castanha-do-pará, atum, canela, grão de bico, granola, pães, entre outros podem ajudar a diminuir as crises de enxaqueca.
+INDICAÇÕES:
+As pessoas com diagnóstico de enxaqueca devem tratar os sintomas de forma correta. Seguir sempre orientação médica e tomar as precauções com relação aos fatores de risco, adotando estilo de vida saudável como atividade física regular, alimentação balanceada e principalmente controlando o peso, pressão arterial e o estresse.
+Alimentos que auxiliam no controle da crise de enxaqueca:
+- Semente de linhaça, atum, sardinha, salmão ou cavala, pois são ricos em ômega 3;
+- Castanhas, amêndoas e amendoim: ricos em selênio, que diminui o estresse;
+- O triptofano ajuda a liberar serotonina, que proporciona sensação de bem-estar. Alimentos como a banana, erva-cidreira, maracujá, pão, arroz, feijão e granola contêm essa substância;
+- Os anti-histamínicos inibem a produção de prostaglandina, responsável pela sensação de dor. São encontrados no orégano, cravo, canela e gengibre;
+- Alguns estudos demonstram que a deficiência de magnésio pode representar um importante papel no desenvolvimento da enxaqueca no período menstrual. Encontrado em amêndoas, avelã, castanha-do-pará, amendoim, alcachofra e espinafre.
+- O consumo de alimentos ricos em vitaminas do complexo B, como feijão, lentilha e grão de bico, também ajuda a prevenir a enxaqueca.
+Alimentos que podem desencadear as crises de enxaqueca:
+- Adoçantes artificiais e produtos diet e light (aspartame e sucralose);
+- Carnes curadas, defumadas, embutidos, salsicha e linguiça, contêm nitratos e nitritos, substâncias que aumentam a dilatação dos vasos sanguíneos;
+- Refrigerantes a base de cola, guaraná, café e o chá mate devem ser evitados, pois possui cafeína, substância estimulante que pode alterar a circulação sanguínea;
+- Bebidas alcoólicas como: vinho tinto, espumantes e destilados em geral possuem fenóis, aldeídos e sulfetos. Essas substâncias podem provocar vasoconstrição dos vasos sanguíneos;
+- Chocolates, queijos duros e frutas cítricas contêm tiramina, substância que libera a prostaglandina, hormônio responsável pela sensação de dor;
+Aditivos alimentares, como o glutamato de monossódico presente em temperos e alimentos industrializados e embutidos.
 CUIDADOS: </t>
+  </si>
+  <si>
+    <t>https://www.hcor.com.br/imprensa/noticias/alimentacao-balanceada-pode-ajudar-contra-as-crises-de-enxaqueca/</t>
+  </si>
+  <si>
+    <t>ALIMENTOS PARA AJUDAR COM PROBLEMAS DE CIRCULAÇÃO
+A má circulação do sangue pode trazer uma série de problemas para a nossa saúde. No entanto, existem alguns alimentos que ajudam na circulação e hoje vamos falar mais sobre isso!
+Para que nossa circulação ocorra adequadamente, é preciso que haja um bom funcionamento do coração, bem como das veias e artérias.
+Todavia, alguns problemas podem atrapalhar a distribuição do sangue em nosso corpo, como o endurecimento dos vasos sanguíneos, o acúmulo de gordura e o mal funcionamento das válvulas destes vasos.
+INDICAÇÕES:
+Consumir alimentos que forneçam as vitaminas e minerais necessários pode ajudar a manter a integridade dos vasos sanguíneos.
+Alguns exemplos destes alimentos são:
+Laranja e outras frutas ricas em vitamina C 
+Frutas ricas em vitamina C e flavonoides possuem ação antioxidante, podendo auxiliar a reduzir o colesterol, um dos inimigos da boa circulação. Além disso, ajudam a fortalecer as paredes dos vasos sanguíneos, contribuindo no bom funcionamento do nosso sistema circulatório. 
+Gengibre
+Esta raiz é um antiinflamatório muito eficaz e combate os problemas circulatórios, pois possui uma enzima que dissolve a fibrina (proteína que participa da coagulação sanguínea). Assim, o gengibre ajuda a afinar o sangue.
+Alho
+Rico em alicina, o alho ajuda a reduzir os níveis de colesterol e triglicérides, prevenindo a obstrução dos vasos sanguíneos.
+Cúrcuma
+A cúrcuma possui a curcumina, que tem poder antioxidante e melhora a resistência dos vasos sanguíneos.
+Salmão, atum, sardinha
+Alimentos ricos em Ômega 3 ajudam a evitar o depósito de gordura nos vasos, auxiliando a circulação e reduzindo a pressão arterial.
+Melão e melancia
+Essas frutas auxiliam a eliminar líquidos e toxinas que podem prejudicar a circulação, como o sódio, por exemplo.
+Uva
+A uva possui substâncias, como os flavonoides, que contribuem para a proteção do coração e para a inibição da formação de trombos sanguíneos.
+Além de todos estes alimentos, devemos lembrar que o consumo de água é um grande aliado para nossa saúde, especialmente para a circulação, uma vez que ajuda na eliminação do sódio e de diversas toxinas do nosso corpo.
+CUIDADOS: É fato que toda essa mudança de hábitos alimentares é extremamente benéfica para a saúde, especialmente se for combinada com a prática de atividades físicas. 
+No entanto, ela não substitui uma visita ao médico, principalmente se você estiver com sintomas que citamos acima e notar que algo não vai bem no seu corpo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM PROBLEMAS DE CONCENTRAÇÃO E MEMÓRIA
+Você já parou para pensar no quanto a alimentação pode influenciar na sua saúde e até nos estudos? A retenção de conteúdo e aumento de concentração podem ser maiores se você tiver qualidade de vida, incluindo boas horas de sono e uma dieta equilibrada, isto é: sem o abuso de certos alimentos como o café e o chocolate, por exemplo.
+INDICAÇÕES:
+Menos salgadinho, mais frutas
+A primeira dica inclui evitar comidas com alta concentração de açúcar e gordura, deixando de lado alimentos ultraprocessados como salgadinhos, bolachas recheadas, sorvetes e refrigerantes. Essas opções são prejudiciais à saúde e pobres em nutrientes. No lugar deles, insira frutas, barrinhas de cereais, torradas integrais ou até leite com aveia. As frutas são essenciais pela função de antioxidante natural, retardando o envelhecimento das células e prevenindo algumas doenças.
+Buscar uma alimentação rica em fibras é fundamental para um bom rendimento nos estudos.
+Ômega 3, Zinco, Colina e Vitaminas do Complexo B estão em alta
+Esses componentes são fundamentais para quem busca uma alimentação equilibrada, ajudando na energia e melhora da memória. Segundo especialistas, o Ômega 3 pode ser encontrado em peixes de água frita, soja, linhaça e frutas; o Zinco em frutos do mar, carnes e gema de ovo e a Colina também em gema de ovo. Já as Vitaminas do Complexo B estão em carnes vermelhas e cereais integrais.
+Na dúvida, coma alface, utilize azeite de oliva e sálvia
+A alface, por ter doses de lactucina em seu talo, principalmente, age como calmante natural, essencial para esta fase. O azeite de oliva, rico em ácidos graxos, auxilia no fortalecimento da memória e a sálvia, como chá ou salada, pode aumentar a concentração em até três horas.
+Hidrate-se
+A ingestão de água, além de melhorar a imunidade, traz benefícios à memória, disposição, auxilia no emagrecimento e na limpeza do organismo. Além disso, a hidratação dificulta o aparecimento de dores de cabeça, náuseas e problemas com a visão – o que é importantíssimo para os momentos de estudo. Por isso, já sabe: pegue sua garrafinha e beba muita água ao longo do dia, ok?
+</t>
+  </si>
+  <si>
+    <t>https://www.sesipr.org.br/colegiosesi/internacional/alimentos-que-melhoram-sua-saude-e-auxiliam-na-concentracao-e-memoria-1-37143-431047.shtml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM PROBLEMAS RESPIRATÓRIOS
+INDICAÇÕES:
+O importante é garantir a eficiência do uso do oxigênio para metabolizar (oxidar) os alimentos. Alimentos muito carregados de carboidratos simples aumentam muito a produção de CO2 e dificultam, forçam muito, o trabalho respiratória. Aumentam demais a acidose do corpo e prejudicam as funções saudáveis.
+1- Comer porções muito grandes de comidas pode cansar, então prefira pequenas porções e com bastante calma e respirando entre as garfadas.
+Comer mais vezes é necessário para atingir a necessidade energética total do dia.
+2- Alimentos que demandam muito trabalho de mastigação podem aumentar o esforço respiratório, então escolha alimentos mais leves, de fácil digestão, se possível mais pastosos, evitando carnes cruas, carnes vermelhas em excesso e carboidratos simples
+3- A escolha dos alimentos é crucial para melhora da eficiência digestiva, de oxidação e absorção dos nutrientes. Deve- se aumentar um pouco o consumo de lipídios saudáveis, proteínas e diminuir carboidratos mais simples. Balancear o prato para ⅓ de salada e legumes cozidos, ¼ para proteínas leves como ovos, peixes e aves é o ideal.
+4- Evite beber durante a refeição, pois líquidos podem diluir o suco gástrico lentificando o trabalho digestivo, aumentando a acidez e refluxo e então, demandando mais trabalho respiratório, o que aumenta o desconforto. É importante que mantenha a hidratação ao longo do dia com preferencialmente água mais alcalina e água de coco, rica em eletrólitos.
+5- A acidificação do corpo prejudica o trabalho pulmonar, então não se deve sobrecarregar a função respiratório com a alimentação. Evite açúcares e farinhas brancas de qualquer origem e beba água com limão (sem açúcar) e consuma vegetais
+6- Sucos, vitaminas e sopas são boas fontes alimentares para aumentar a densidade de nutrientes sem forçar demais o sistema pulmonar. Sucos verde são boas opções para incrementar os nutrientes a função destoxificação do corpo, incluindo a via pulmonar
+Para melhorar o aporte proteico, pode incluir nos shakes a clara de ovo cozida.
+7- Consuma alimentos fontes de Ferro (carnes bovina, porco e aves e peixes mais escuros, feijões, folhas verde escuras e ervas frescas). O ferro é crucial para garantir a oxigenação do corpo. E alimentos fonte de vitamina C (limão, tangerina, acerola, caju, goiaba, goji…) que garantem a melhor absorção do ferro no corpo.
+8- Consuma maior parte da energia do dia em gorduras saudáveis como iogurtes, queijos maturados, óleos como azeite de oliva, de castanhas e sementes, sempre extravirgens. Consuma castanhas e frutas como coco, azeitona e abacate, Óleo de coco e Manteiga com moderação.
+9- Importante fortalecer o sistema imunológico, já que o defesa das vias aéreas podem estar mais comprometidas. Então consuma, probióticos, probióticos, alho, cebola, cogumelos, algas, levedo
+10- Infusões fitoterápicos de gengibre, alecrim, hortelã, limão, canela, guaco e outras calmantes como camomila, Melissa e lavanda, ajudam na melhora respiratória.
+Assim como a fitoterapia, a aromaterapia é super bem vinda; fazer ciclos de inspiração e expiração sob o sol em contato com a natureza e com aromas de hortelã, eucalipto, casca de limão, lavanda, sândalo vão melhorar muito a percepção da função respiratória.
+11- Suplementos podem ser administrados para diminuir o potencial inflamatório, para melhorar sistema imunológico, alcalinizar e garantir destoxificação do corpo. Para dar suporte de proteínas e fosfolipídeos importantes para constituição do muco e surfactante pulmonar.
+Antioxidante para garantir o combate às agressões das toxinas as quais somos expostos e para otimizar o tratamento medicamentoso. Os antioxidantes encontrados naturalmente no trato respiratório inferior são: superóxido dismutase, catalase e glutationa), juntamente com a ceruloplasmina, cobre, metionina sulfóxido, retinóides e vitaminas E e C, assim, pode-se pensar em sua suplementação complementar.
+Eletrólitos e minerais necessários ao trabalho de contração celular e portanto, eficiência da função respiratória como magnésio, potássio, fósforo, cloreto e sódio devem ser levados em consideração.
+O mais importante na dieta do paciente com disfunção respiratória é garantir os porte energética necessário para o dia e sua hidratação.
+</t>
+  </si>
+  <si>
+    <t>https://espacodevida.org.br/dicas-de-alimentacao-para-quem-esta-com-insuficiencia-respiratoria-de-qualquer-causa/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A GRIPE
+A queda da temperatura e a proximidade do inverno gera apenas uma certeza ao brasileiro: lá vem a gripe! A época é de maior circulação de vírus respiratórios e, o único meio de prevenção, é a vacinação. No entanto, uma vez instalado o quadro, além dos medicamentos, é possível aliviar os sintomas e melhorar a imunidade por meio da dieta.
+INDICAÇÕES:
+Entre o que deve ser evitado, estão as bebidas alcoólicas, alimentos ricos em gorduras e açúcar, laticínios, frituras e cafeína em excesso. Isso porque esses alimentos podem interferir na hidratação corporal e aumentar o processo inflamatório. Carla Falsete, otorrinolaringologista pela ABORL-CCF (Associação Brasileira de Otorrinolaringologia e Cirurgia Cérvico-Facial) explica que alguns desses alimentos, ainda, podem aumentar a produção de muco e, consequentemente, o congestionamento nasal, dificultando a respiração.
+Os alimentos que são consenso entre os especialistas são aqueles ricos em vitamina C – entre eles as frutas cítricas e vegetais verdes folhosos. Isso porque a vitamina C aumenta a produção de glóbulos brancos, essenciais no combate às infecções. Podem ser destacados a laranja, o limão, kiwi, acerola e o tomate Thais elenca ainda alguns alimentos que ajudam na recuperação. Peixes e ovos são boas fontes de vitamina D, que ajudam a regular e fortalecer o sistema imunológico. Carnes magras e legumes são ricos em zinco, crucial para o funcionamento normal do sistema imunológico. Nozes e sementes contêm vitamina E, um antioxidante poderoso que ajuda a manter o sistema imunológico saudável.
+Se destaca, também, o mel. Isso porque ele tem ação antitussígena, auxiliando na melhora deste sintoma. É recomendado, ainda, que seja ingerida uma grande quantidade de líquidos e que o paciente repouse para melhor recuperação do quadro gripal.
+Ainda, segundo a endocrinologista, o iogurte contém probióticos, que são bactérias benéficas que podem melhorar a saúde do intestino, onde muitas das células imunológicas do corpo são encontradas. Já o alho e o gengibre têm propriedades anti-inflamatórias e antimicrobianas que podem ajudar a fortalecer a resistência do corpo a infecções.
+</t>
+  </si>
+  <si>
+    <t>https://www.hospitaloswaldocruz.org.br/imprensa/hospital-na-midia/bateu-a-gripe-veja-os-alimentos-que-ajudam-a-melhorar-a-imunidade-e-combater-a-doenca/</t>
+  </si>
+  <si>
+    <t>ALIMENTOS PARA AJUDAR COM A FEBRE
+Pode ser bastante incomodativa, mas tem uma razão de ser. Existem algumas estratégias para ajudar a baixar a febre e diminuir o mal-estar que possa causar.
+A febre (ou hipertermia) pode ser bastante incomodativa, mas na maior parte dos casos, representa uma resposta normal e temporária do nosso organismo na tentativa de combater inflamações e infeções. Considera-se que uma pessoa tem febre quando a sua temperatura corporal está cerca de 1ºC acima da temperatura habitual (entre 36 e 37ºC), embora possa variar de indivíduo para indivíduo. Ainda que seja um mecanismo natural do nosso sistema imunitário, há estratégias que podemos adotar para diminuir o desconforto que a febre pode provocar e favorecer a recuperação.
+Nos adultos, a febre pode provocar:
+Dor de cabeça
+Suores
+Fraqueza
+Arrepios
+Dor muscular
+Desidratação
+Falta de apetite
+Febre muito alta pode provocar também confusão mental, cansaço extremo, irritabilidade, tonturas e convulsões.
+INDICAÇÕES:
+Beba muita água, sumos e caldos: a febre pode levar à perda de fluidos corporais, o que, por sua vez, pode favorecer a desidratação. A ingestão de líquidos ajuda também a baixar a temperatura corporal.
+Prefira alimentos fáceis de digerir.
+Descanse e evite atividades intensas que possam aumentar a temperatura corporal, atrasando a recuperação.
+Tome um banho morno (não frio) ou aplique toalhas húmidas na testa e pulsos.
+Vista roupa leve (mesmo que sinta arrepios), mantenha a temperatura ambiente fresca e diminua a quantidade de roupa de cama.
+Tome os medicamentos antipiréticos recomendados pelo seu médico assistente.
+CUIDADOS: A febre por si só não implica necessariamente uma visita ao seu médico assistente. Deverá, sim, fazê-lo em caso de:
+Febre superior a 40ºC
+Febre persistente por mais de três dias ou que não melhora com antipiréticos
+Dor de cabeça
+Rigidez no pescoço e dor quando dobra a cabeça para a frente
+Sensibilidade anormal à luz intensa
+Dor de garganta persistente e/ou dificuldade em engolir
+Inchaço, inflamação ou dor severa nalguma zona do corpo
+Manchas na pele de aparecimento recente
+Confusão mental
+Vómitos
+Dificuldade em respirar ou dor no peito
+Cansaço ou irritabilidade inexplicáveis
+Urina mais escura do que o habitual ou dor ao urinar
+Perda de consciência
+Tonturas
+Viagem recente ao estrangeiro</t>
+  </si>
+  <si>
+    <t>https://www.cuf.pt/mais-saude/o-que-fazer-para-baixar-febre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM CONTUSÕES
+Ninguém consegue ficar imune às lesões, porque podem acontecer a qualquer hora e em qualquer lugar. Os atletas têm mais chance de se lesionar do que as pessoas que não são atletas em função da atividade desportiva.
+INDICAÇÕES:
+   Para recuperar e até mesmo prevenir lesões, os alimentos podem ser grandes aliados. Uma nutrição adequada é muito importante para a recuperação dos tecidos. Alimentos que sejam ricos em antioxidantes, fatores anti-inflamatórios e aminoácidos, vão ajudar o corpo a se fortalecer, reconstruir o colágeno e os tecidos. 
+   Um nutriente fundamental neste processo são as gorduras, como ômega 3 e ácidos graxos que diminuem a dor e reduzem a inflamação, fator este que atrasa a recuperação de tendinites, de fraturas ósseas e de torções de ligamentos.
+   Apostar em alimentos ricos em vitamina C (laranja, limão, mirtilo, morangos) auxilia no processo de regeneração da pele, na reparação do tecido cicatricial, dos tendões, dos ligamentos e dos vasos sanguíneos. A vitamina D é importante para a saúde óssea e para a absorção de cálcio, podendo ser obtida com a exposição solar protegida e moderada. Ambos micronutrientes atuam favoravelmente na hora de recuperar e estimulam a proteção do sistema imunitário, deixando-o mais capaz de agir contra os marcadores de inflamação. 
+   A boa hidratação diminui o estresse do organismo. Tecidos e articulações desidratadas possuem maior dificuldade para lutar contra a agressão, eliminar toxinas e reparar danos.
+   O adequado consumo proteico é um elemento fundamental para a produção de novas células e para a saúde muscular, melhorando a síntese proteica. A ingestão de alimentos que sejam reconstrutores, ou anticatabólicos, ajudam a evitar a perda de tecido muscular. As proteínas pode vir de ovos, peixes, carnes vermelhas ou brancas, tofu, quinoa, cogumelos, leguminosas...
+   Alimentos ricos em zinco, tais como nozes, grãos e frango vão ajudar seu corpo a usar as gorduras e proteínas presentes na sua alimentação para reparar o tecido lesionado, além de fortalecer o sistema imunológico.
+</t>
+  </si>
+  <si>
+    <t>https://www.physiomet.com.br/blog/como-a-alimentacao-pode-ajudar-na-recuperacao-das-lesoes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A ARTROSE
+Conhecida também como artrite degenerativa, artrose é uma doença reumática, que afeta as articulações, limitando  movimentos e que não tem cura, somente tratamento. Atinge principalmente os joelhos, coluna, quadril, mãos e dedos. Pode manifestar-se em pessoas de ambos os sexos e de qualquer idade, aumentando a incidência com o passar dos anos. As causas são devido a fatores genéticos, imunidade baixa, obesidade e atividades repetitivas que causam sobrecarga nas articulações. O principal sintoma é a dor, ocorrendo com a movimentação da articulação afetada.
+INDICAÇÕES:
+É importante evitar certos “alimentos” que são na verdade produtos alimentícios, como: fastfood, comidas congeladas, embutidos, enlatados, caldos e tabletes de tempero, açúcar, xarope de milho/guaraná, bebidas gaseificadas (refrigerante), gordura hidrogenada, sucos de pó e caixinha, leite e derivados; enfim, quase tudo que tenha vida de prateleira e rótulo. Tudo que for doce e gordo ao mesmo tempo não é alimento de verdade.
+Então as pessoas se perguntam: o que comer ? A resposta é simples: COMIDA DE VERDADE.
+Os alimentos (legumes, verduras, frutas, grãos integrais, ovo caipira) possuem nutrientes que tem função terapêutica e ao serem consumidos por um longo período, auxiliam no tratamento e na melhora do quadro sintomático, inflamatório e imunológico da doença.   A obesidade é um fator de risco para quem possui artrose podendo contribuir lesionando ainda mais as articulações, neste caso a alimentação saudável auxilia não somente na modulação do estress oxidativo da doença, mas também no gerenciamento do peso  tornando-se importante na melhora da superfície articular comprometida.
+A alimentação natural é a mais indicada, comida orgânica (sem agrotóxico), frutas e legumes da época (safra), horta caseira, colheita da roça, ovo de galinha que cisca, leite e  queijo da vaquinha feliz (só se alimenta de capim e ração natural); isso sim traz saúde.
+A ingestão de alimentos fonte de ômega 3 como os peixe  sardinha e cavalinha, chia, Linhaça triturada e até mesmo a suplementação via oral do ácido graxo em questão é uma boa pedida para a  melhora do processo inflamatório. Fontes de vitamina D e cálcio são importantes para evitar a desmineralização óssea comum no estágio avançado da doença e para manutenção da saúde imunológica. Vitaminas do complexo B, Vitamina C e Vitamina E são requisitadas para gerenciamento do estresse oxidativo, melhora do metabolismo da glicose e controle de peso.
+Sucos detox (couve, cenoura, gengibre, maça, limão, água) têm ação alcalina, vão diminuir o depósito de substâncias nas articulações e melhorar a disbiose intestinal (alteração na quantidade e na qualidade das bactérias intestinais).  É indicado o aumento da ingestão diária de ervas naturais como alecrim, salsinha, cebolinha, manjericão, orégano, louro, páprica, pimenta do reino (antioxidantes);  alho e cebola (anti inflamatórios); Banana ( fonte de vitamina B6 e triptofano- diminui dores e ansiedade); Biomassa de Banana Verde, Kefir, kombuchá , Batata Yakón (prebióticos); Laranja lima (melhora o sistema imunológico), Castanha do Pará ( fonte de selênio- ativa sistema de defesa- Glutationa); Mamão (enzima digestiva- papaina); Abacaxi (enzima digestiva- bromelina); enfim alimentos de verdade.
+Artrose não tem cura, mas existem várias medidas a serem tomadas, dependendo do caso exercícios físicos podem diminuir ou aumentar a dor, e em alguns casos há progresso com repouso. Medicação, Nutrição (alimentação), Fisioterapia e Saúde mental (Reiki, Yoga, Meditação) são tratamentos que colaboram com a melhora do quadro clínico e qualidade de vida.
+</t>
+  </si>
+  <si>
+    <t>https://encontrar.org.br/uma-boa-nutricao-pode-auxiliar-no-combate-aos-sintomas-da-artrose/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A ARTRITE
+Estudos confirmam que o consumo de alimentos comuns na dieta mediterrânea traz os seguintes benefícios:
+• Reduz a pressão arterial
+• Protege contra doenças crônicas, desde câncer até AVC
+• Auxilia no tratamento da artrite, diminuindo a inflamação
+• Beneficia as articulações e o coração
+• Leva à perda de peso, o que pode reduzir a dor nas articulações  
+INDICAÇÕES:
+- Peixe
+Quantidade:  Autoridades de saúde como a Associação Americana do Coração e a Academia de Nutrição e Dietética recomendam de 85 a 115 gramas de peixe, duas vezes por semana. Especialistas em artrite afirmam que quanto mais, melhor.
+Porquê:  Alguns tipos de peixe são boas fontes de ácidos graxos ômega-3, que combatem a inflamação. Um estudo descobriu que aqueles que consumiam mais ômega-3 apresentavam níveis mais baixos de duas proteínas inflamatórias: proteína C-reativa (PCR) e interleucina-6. Mais recentemente, pesquisadores demonstraram que a ingestão de suplementos de óleo de peixe ajuda a reduzir o inchaço e a dor nas articulações, a duração da rigidez matinal e a atividade da doença em pessoas com artrite reumatoide (AR).
+Melhores fontes:  Salmão, atum, sardinha, arenque, anchova, vieira e outros peixes de água fria. Não gosta de peixe? Tome um suplemento. Estudos mostram que a ingestão diária de 600 a 1.000 mg de óleo de peixe alivia a rigidez, a sensibilidade, a dor e o inchaço nas articulações.
+- Nozes e sementes
+Quantidade:  Consuma 42,5 gramas de nozes por dia (30 gramas equivalem a aproximadamente um punhado).
+Porquê:  “Diversos estudos confirmam o papel das nozes em uma dieta anti-inflamatória”, explica José M. Ordovás, PhD, diretor de nutrição e genômica do Centro de Pesquisa em Nutrição Humana Jean Mayer do USDA sobre Envelhecimento, na Universidade Tufts, em Boston. Um estudo constatou que, ao longo de um período de 15 anos, homens e mulheres que consumiram mais nozes apresentaram um risco 51% menor de morrer de uma doença inflamatória (como artrite reumatoide) em comparação com aqueles que consumiram menos nozes. Outro estudo descobriu que indivíduos com níveis mais baixos de vitamina B6 — encontrada na maioria das nozes — apresentavam níveis mais altos de marcadores inflamatórios.
+Mais boas notícias:  as nozes são repletas de gordura monoinsaturada, que combate a inflamação. E embora sejam relativamente ricas em gordura e calorias, estudos mostram que o consumo de nozes promove a perda de peso porque suas proteínas, fibras e gorduras monoinsaturadas são saciantes. "Lembre-se apenas de que mais nem sempre é melhor", diz Ordovás.
+Melhores fontes:  Nozes, pinhões, pistaches e amêndoas.
+- Frutas e Vegetais
+Quantidade:  Procure consumir nove ou mais porções por dia (uma porção equivale a uma xícara da maioria dos vegetais ou frutas, ou duas xícaras de folhas verdes cruas).
+Porquê:  Frutas e vegetais são ricos em antioxidantes. Esses compostos químicos potentes atuam como o sistema de defesa natural do corpo, ajudando a neutralizar moléculas instáveis ​​chamadas radicais livres, que podem danificar as células. Pesquisas demonstraram que as antocianinas encontradas em cerejas e outras frutas vermelhas e roxas, como morangos, framboesas, mirtilos e amoras, têm efeito anti-inflamatório.
+Mais boas notícias:  frutas cítricas — como laranjas, toranjas e limões — são ricas em vitamina C. Pesquisas mostram que ingerir a quantidade adequada dessa vitamina ajuda a prevenir a artrite inflamatória e a manter as articulações saudáveis. Outras pesquisas sugerem que o consumo de vegetais ricos em vitamina K, como brócolis, espinafre, alface, couve e repolho, reduz drasticamente os marcadores inflamatórios no sangue.
+Melhores fontes:  Frutas e vegetais coloridos — quanto mais escura ou brilhante a cor, mais antioxidantes eles contêm. Boas opções incluem mirtilos, cerejas, espinafre, couve e brócolis.
+- Azeite
+Quantidade:  Duas a três colheres de sopa por dia.
+Porquê:  O azeite é rico em gorduras saudáveis ​​para o coração, bem como em oleocantal, que possui propriedades semelhantes aos anti-inflamatórios não esteroides (AINEs). "O oleocantal inibe a atividade das enzimas COX, com uma ação farmacológica semelhante à do ibuprofeno", afirma Ordovás. A inibição dessas enzimas atenua os processos inflamatórios do organismo e reduz a sensibilidade à dor.
+Melhores fontes:  O azeite extra virgem passa por menos refinamento e processamento, retendo assim mais nutrientes do que as variedades comuns. E não é o único óleo com benefícios para a saúde. Os óleos de abacate e cártamo demonstraram propriedades redutoras do colesterol, enquanto o óleo de noz possui 10 vezes mais ômega-3 do que o azeite.
+- Feijões
+Quantidade:  Cerca de uma xícara, duas vezes por semana (ou mais).
+Porquê:  Os feijões são ricos em fibras e fitonutrientes, que ajudam a reduzir a PCR (proteína C-reativa), um indicador de inflamação presente no sangue. Níveis elevados de PCR podem indicar desde uma infecção até artrite reumatoide. Num estudo, cientistas analisaram o conteúdo nutricional de 10 variedades comuns de feijão e identificaram diversos compostos antioxidantes e anti-inflamatórios. Os feijões também são uma excelente e barata fonte de proteína, com cerca de 15 gramas por xícara, o que é importante para a saúde muscular.
+Melhores fontes:  Feijões vermelhos pequenos, feijões vermelhos e feijões carioca estão entre os quatro principais alimentos com alto teor de antioxidantes, segundo o Departamento de Agricultura dos EUA (mirtilos silvestres ocupam o segundo lugar).
+- Grãos integrais
+Quantidade:  Consuma um total de seis onças (aproximadamente 170 gramas) de grãos por dia; pelo menos três dessas onças devem ser de grãos integrais. Uma onça (aproximadamente 28 gramas) de grãos integrais equivale a ½ xícara de arroz integral cozido ou uma fatia de pão integral.
+Porquê:  Os grãos integrais contêm muita fibra, que dá saciedade e pode ajudar a manter um peso saudável. Alguns estudos também mostraram que  a fibra  e os alimentos ricos em fibras podem reduzir os níveis sanguíneos de PCR, um marcador inflamatório. 
+Melhores fontes:  Consuma alimentos feitos com o grão inteiro, como farinha de trigo integral, aveia, bulgur, arroz integral e quinoa. Algumas pessoas podem precisar ter cuidado com os grãos integrais que consomem.  O glúten  — uma proteína encontrada no trigo e em outros grãos — tem sido associado à inflamação em pessoas com doença celíaca ou sensibilidade ao glúten. 
+- Vegetais da família das solanáceas
+Porquê:  Os vegetais da família das solanáceas , incluindo beringela, tomate, pimentão vermelho e batata, são verdadeiras potências no combate a doenças, oferecendo o máximo de nutrientes com o mínimo de calorias.
+Por que não?  Elas também contêm solanina, uma substância química que tem sido apontada como a culpada pelas dores da artrite. Não há evidências científicas que sugiram que as solanáceas desencadeiem crises de artrite.
+Faça o teste:  Alguns especialistas acreditam que esses vegetais contêm uma poderosa combinação de nutrientes que ajuda a inibir a dor da artrite. No entanto, muitas pessoas relatam alívio dos sintomas ao evitar vegetais da família das solanáceas. Portanto, se você notar que a dor da sua artrite piora depois de consumi-los, considere eliminar todos os vegetais da família das solanáceas da sua dieta por algumas semanas para ver se faz diferença. Depois, reintroduza-os lentamente na sua dieta para observar se os sintomas pioram ou permanecem os mesmos.
+</t>
+  </si>
+  <si>
+    <t>https://www.arthritis.org/health-wellness/healthy-living/nutrition/anti-inflammatory/the-ultimate-arthritis-diet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM CISTITE
+Uma dieta equilibrada, com uma grande variedade de alimentos de todos os grupos alimentares, é a melhor dieta para a síndrome da bexiga dolorosa/cistite intersticial.
+INDICAÇÕES:
+Os nutrientes dos alimentos ajudam a fortalecer o sistema imunológico, cicatrizar feridas, estimular a transmissão nervosa, manter o fluxo sanguíneo normal e promover a saúde em geral. Uma dieta equilibrada, com uma grande variedade de alimentos de todos os grupos alimentares, é a melhor dieta para cistite intersticial/síndrome da bexiga dolorosa (CI/SBD). É também a melhor dieta para todos. A única diferença é que pessoas com CI/SBD devem limitar o consumo de alguns alimentos e bebidas.
+Restringir demais alimentos e bebidas pode afetar negativamente o seu bem-estar. Por isso, é muito importante substituir os nutrientes fornecidos por alimentos e bebidas problemáticos por opções alternativas. Felizmente, é fácil encontrar alimentos e bebidas que podem substituir aqueles que precisam ser restringidos para ajudar a controlar os sintomas da bexiga. Para obter a nutrição necessária:
+Procure consumir uma variedade de alimentos.
+Coma com moderação — muitas vezes os restaurantes servem porções maiores do que você precisa. Então, peça para levar o que sobrou para casa!
+Beba bastante líquido — urine e depois dê uma olhada; sua urina deve estar com uma cor amarelo-clara.
+Controle o consumo de açúcar, sal, álcool e gordura (especificamente gordura saturada, gordura trans e colesterol proveniente de produtos de origem animal e processados). Essas recomendações valem para todos.
+Verifique o rótulo de informações nutricionais e a lista de ingredientes para saber as quantidades de gordura saturada, sódio e açúcares adicionados nos alimentos e bebidas que você escolher, bem como os itens que desencadeiam sua cistite intersticial/síndrome da bexiga dolorosa.
+</t>
+  </si>
+  <si>
+    <t>https://www.ichelp.org/understanding-ic/diet/what-to-eat/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM MENSTRUAÇÃO IRREGULAR
+INDICAÇÕES:
+Uma dieta anti-inflamatória prioriza o consumo de alimentos minimamente processados. Alimentos ricos em fibras, vitaminas e minerais podem ajudar a reduzir a inflamação, além de contribuir para o equilíbrio hormonal.
+Os vegetais  são ricos em fibras, fitonutrientes, vitamina C, folato e magnésio. As fibras vegetais ajudam a alimentar as bactérias benéficas do intestino e promovem a regularidade intestinal. Quando o intestino apresenta o equilíbrio correto de bactérias e o trato gastrointestinal funciona adequadamente, a inflamação diminui. Vegetais folhosos verdes são uma excelente fonte de magnésio. O magnésio é importante para reduzir a inflamação e manter o equilíbrio hormonal, auxiliando na produção de insulina e hormônios da tireoide, além de contribuir para a produção de estrogênio e progesterona.
+Os fitoestrogênios  são um tipo de fitonutriente encontrado em alimentos como nozes, leguminosas, grãos integrais, linhaça e soja. Os fitoestrogênios podem diminuir a eficácia do estrogênio. Isso pode ser útil se você tiver sintomas de excesso de estrogênio, como menstruação intensa, sensibilidade mamária, TPM ou miomas.
+A proteína  é muito importante para manter a massa muscular magra e fornecer aminoácidos essenciais para a reparação dos órgãos. Ela também é necessária para manter o equilíbrio hormonal. O fígado é responsável por eliminar o excesso de hormônios. Os aminoácidos (os blocos de construção das proteínas) são necessários para "empacotar" as toxinas, para que possam ser eliminadas do corpo. Você deve ingerir pelo menos 1 grama de proteína para cada quilograma do seu peso corporal ideal. Por exemplo, se você pesa 68,2 kg (divida 68,2 kg por 2,2 kg para obter 68,2 kg), você precisa de pelo menos 68 gramas de proteína. A  proteína animal também é uma excelente fonte de zinco. O zinco é necessário para o desenvolvimento dos folículos. Ele também regula o eixo HPA e tem benefícios anti-inflamatórios. Como o corpo não armazena zinco, ele precisa ser obtido diariamente por meio da alimentação. Ao escolher proteína animal, é melhor optar por aves criadas soltas e minimamente processadas, carne de animais alimentados a pasto, peixes selvagens e laticínios e ovos orgânicos.
+Dietas vegetarianas e veganas  ricas em vegetais, carboidratos complexos e diversas fontes de proteína ajudam a manter um ciclo menstrual regular. Às vezes, pode ser difícil obter proteína suficiente em uma dieta vegetariana ou vegana. Isso pode levar a desequilíbrios hormonais. Menstruações irregulares também podem ser causadas por deficiência de zinco. O consumo frequente de soja e leguminosas pode levar ao consumo excessivo de fitoestrogênios. Embora benéficos, o excesso de fitoestrogênios pode bloquear a ovulação.
+Os carboidratos complexos  são carboidratos de digestão lenta que fornecem energia ao corpo. Eles também contêm fibras e amido, que alimentam as bactérias benéficas do intestino. Os carboidratos também são necessários para a ativação do hormônio da tireoide e podem diminuir o cortisol. Recomenda-se consumir cerca de 150 a 200 gramas de carboidratos por dia para manter um ciclo menstrual saudável.
+Muitas mulheres experimentam dietas com baixo teor de carboidratos na tentativa de perder peso. Algumas mulheres têm sucesso com essas dietas. Outras descobrem que dietas com baixo teor de carboidratos afetam negativamente seu ciclo menstrual. Se você sofre de ansiedade, insônia, queda de cabelo, constipação, ausência de menstruação ou estagnação na perda de peso, pode se beneficiar da inclusão de carboidratos complexos em sua dieta .
+As gorduras  são os componentes básicos do estrogênio e da progesterona. A ingestão insuficiente de gordura pode causar menstruação irregular ou intensa, TPM ou anovulação. É melhor optar por gorduras de origem vegetal com mais frequência do que por gorduras de origem animal. As gorduras insaturadas presentes nas gorduras vegetais contribuem para a saúde do sistema cardiovascular.
+As gorduras ômega-3  são um tipo especial de gordura encontrada no óleo de coco, em peixes e em ovos orgânicos. As gorduras ômega-3 são anti-inflamatórias e desempenham um papel importante na redução da inflamação no corpo.
+A vitamina D  desempenha diversas funções. Ela regula mais de 200 genes e é essencial para o metabolismo e a ovulação. A melhor fonte de vitamina D é o sol. No entanto, a falta de exposição solar, a obesidade, a inflamação crônica e a deficiência de magnésio podem impedir o organismo de obter vitamina D suficiente. A recomendação geral é de 2000 UI de vitamina D por dia. Converse com seu médico sobre a possibilidade de fazer um exame para verificar seus níveis de vitamina D e determinar a dose adequada de suplemento para você.
+</t>
+  </si>
+  <si>
+    <t>https://femalehealthawareness.org/en/nutritional-considerations-for-a-healthy-menstrual-cycle/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A CÓLICA
+INDICAÇÕES:
+Como aliviar a cólica menstrual: métodos naturais e caseiros
+Algumas medidas simples e seguras podem ajudar a reduzir a dor e proporcionar mais conforto durante o período menstrual:
+1. Aplicação de calor
+O uso de bolsas térmicas mornas sobre a região abdominal ajuda a relaxar os músculos do útero e melhora o fluxo sanguíneo, aliviando as contrações dolorosas.
+2. Chás com efeito calmante e anti-inflamatório
+Algumas infusões naturais são aliadas no combate à cólica:
+Camomila: tem ação calmante e ajuda a relaxar o corpo.
+Erva-doce: possui efeito antiespasmódico, ou seja, reduz as contrações.
+Gengibre: atua como anti-inflamatório natural, aliviando a dor.
+Esses chás devem ser consumidos com moderação e sem adoçantes em excesso.
+3. Técnicas de relaxamento
+Respirar profundamente, praticar meditação ou tomar um banho morno pode diminuir a tensão muscular e mental, favorecendo o alívio da dor. O equilíbrio emocional também tem papel importante no controle da percepção da dor.
+- Alimentos que ajudam a reduzir a cólica menstrual
+A alimentação tem impacto direto na intensidade das cólicas. Durante o ciclo, é importante priorizar:
+Fontes de magnésio, como banana, espinafre, abacate e sementes;
+Alimentos ricos em ômega-3, como peixes, linhaça e chia, que têm ação anti-inflamatória;
+Fibras naturais, presentes em frutas, legumes e grãos integrais, que favorecem o funcionamento intestinal e reduzem o inchaço.
+- Evitar certos alimentos também pode ajudar, especialmente:
+Cafeína (café, refrigerantes e alguns chás escuros), que pode aumentar a sensibilidade à dor;
+Frituras e alimentos ultraprocessados, que favorecem processos inflamatórios;
+Excesso de sal, que contribui para retenção de líquidos e desconforto abdominal.
+</t>
+  </si>
+  <si>
+    <t>https://hospitalsiriolibanes.org.br/blog/ginecologia/dicas-colica-menstrual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM TENSÃO PRÉ-MENSTRUAL
+A Tensão Pré-Menstrual está no calendário. Não tem jeito, já que a TPM faz parte do ciclo natural do corpo da mulher. Com ela, chegam sintomas como ataques de nervos, inchaço, cólicas, dores de cabeça, irritabilidade e choro fácil. E tudo vai embora com a chegada da menstruação. Mas é preciso saber que existem formas de encarar melhor o processo.
+INDICAÇÕES:
+Uma boa alimentação é importante. Entre as dicas, estão o consumo de comidas leves, e muita água e chás. Segundo Márcia Gaspar Nunes, doutora do Departamento de Ginecologia da Unifesp, é bem comum a indicação de alimentos como oleaginosas, cacau, banana e aveia. E os efeitos no organismo da mulher têm base científica.
+CINCO ALIMENTOS
+1. Oleaginosas (feijão, lentilha, ervilhas...)
+2. Banana
+3. Aveia
+4. Peixes de mar profundo
+5. Verduras escuras
+"A síndrome da TPM é um monte de sintomas misturados. São mais de 150 descritos e é muito comum sentir esses efeitos da menstruação. A alimentação pode ajudar para quadros moderados, que chegam a atingir 40% de mulheres, mas um grupo bem pequeno tem a forma grave e é preciso buscar tratamento", ressalta a doutora.
+A sugestão de mudança na dieta vai ajudar as mulheres por conta das mudanças hormonais características do período menstrual. A regulação dos neurotransmissores no cérebro é afetada e alimentos ricos em determinadas vitaminas e minerais pode colaborar para estabilizar as membranas neuronais e criar neurotransmissores.
+O triptofano tem um papel importante na transformação serotonina e os alimentos ricos na substância têm um ótimo desempenho colaborando para melhorar o humor. Entre eles, estão oleaginosos (feijão, ervilhas, amendoim e lentilhas), aves, nozes e sementes e peixes (atum, linguado, salmão, sardinha e bacalhau).
+A banana também é importante, pois é rica na vitamina B6, que é parte da produção da serotonina. A fruta ainda tem alguns outros micronutrientes que podem ajudar durante o período. Um exemplo é o magnésio, que atua na estabilização da membrana cerebral e auxilia na produção de insulina pelo pâncreas.
+O cálcio também é importante, já que contribui com a contração muscular, na transmissão impulso nervoso e no acúmulo de energia dentro da célula. Duas fontes do recurso são as verduras (as mais verdes, como couve e brócolis) e laticínios. Mais um item que ajuda no combate aos sintomas da TPM é o Ômega 3.
+Segundo a doutora Márcia, a substância, encontrada em peixes do mar profundo, como sardinha, atum e bacalhau, colaboram com a plasticidade cerebral e acabam tendo um efeito positivo em todo o contexto. Além dos alimentos que ajudam, também é importante que as mulheres estejam atentas a hábitos que atrapalham.
+A vontade maior que o costume para o consumo de doces deve ser evitada. "Em vez de, no lanche, ir à padaria comer um quindim, é melhor fazer um lanche rápido com castanha do Pará, por exemplo, que é rica triptofano e vai ajudar a combater os transtornos de humor causados pela TPM", aconselha.
+Deixar de lado
+Também é importante dar um tempo em bebidas que contenham cafeína (como café e energético) e até dar um tempo no álcool. Isso porque eles têm um efeito irritantes. Os alimentos ricos em sódio também não são uma boa, já que contribuem para o acúmulo de líquido pelo organismo, algo que já é potencializado pela TPM.
+</t>
+  </si>
+  <si>
+    <t>https://www.gov.br/saude/pt-br/assuntos/saude-brasil/eu-quero-me-alimentar-melhor/noticias/2018/cinco-alimentos-para-enfrentar-melhor-a-tpm</t>
+  </si>
+  <si>
+    <t>ALIMENTOS PARA AJUDAR COM QUEIMADURAS
+INDICAÇÕES:
+Uma dieta equilibrada é a melhor maneira de garantir sua nutrição adequada. Se as queimaduras ainda estiverem abertas, sua dieta deve incluir proteína extra. À medida que você continua a se recuperar, suas necessidades nutricionais voltarão a ser como eram antes da lesão. Agora é importante focar em uma dieta equilibrada. Evite alimentos com pouco valor nutricional, como bebidas açucaradas, sobremesas, doces, carnes gordas e pães ou biscoitos brancos. Consuma mais carnes magras, grãos integrais, vegetais, frutas e laticínios com baixo teor de gordura.
+Faça pequenas refeições e lanches frequentes para evitar sentir tanta fome a ponto de comer demais de uma só vez.
+Inclua proteína em todas as refeições e lanches. A proteína ajuda a manter a sensação de saciedade e a fortalecer o corpo. Boas fontes de proteína são carne bovina, frango, carne suína, ovos, feijão, nozes, leite, iogurte e queijo.
+Corte frutas e vegetais em fatias para um lanche rápido e prático. Eles fornecem muitos nutrientes essenciais para a recuperação e a saúde em geral.
+Varie os sabores dos alimentos que você come para mantê-los saborosos e interessantes. Cozinhe com especiarias e ervas, como alecrim, hortelã, alho, pimenta caiena e manjericão.
+Beba água durante o dia para se manter hidratado e evitar calorias desnecessárias. Muitas bebidas contêm gordura e açúcar que seu corpo não precisa. Leia as informações nutricionais nos rótulos dos alimentos.
+Escolha pães integrais e outros alimentos ricos em fibras. Eles ajudam a manter a sensação de saciedade entre as refeições e podem contribuir para o funcionamento regular do intestino.
+Procure comer apenas quando estiver com fome. Evite comer por outros motivos, como tédio, falta de controle, raiva ou desesperança. Mantenha um diário alimentar e monitore seu humor para verificar se sua alimentação está relacionada às suas emoções.
+CUIDADOS: Converse com seu médico sobre quaisquer vitaminas e suplementos que você gostaria de tomar em casa.</t>
+  </si>
+  <si>
+    <t>https://msktc.org/burn/factsheets/healthy-eating-after-burn-injury-adults</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM DERMATITES
+INDICAÇÕES:
+Peixe: Os ácidos gordos ómega 3 encontrados no peixe, como no salmão, atum, sardinhas ou mesmo no marisco, possuem propriedades anti-inflamatórias que combatem os danos causados pela exposição prolongada ao sol. Legumes folhas verdes: A vitamina A combate o envelhecimento precoce, a formação de escamas e a desidratação. Também é essencial para a renovação celular e promove o crescimento de nova pele. “Os espinafres e brócolis, por exemplo, são excelentes fontes de vitamina A”. Citrinos: A vitamina C é um antioxidante muito poderoso que pode manter o colágeno na estrutura da pele e impedir a flacidez. “Laranjas, mexericas, limões e limas são também excelentes escolhas”.
+Água:  a água estimula o trânsito intestinal e a eliminação de toxinas do organismo, impedindo que o seu acúmulo seja refletido na pele. “A ingestão recomendada é de oito copos ou 2 litros/dia. Se não houver boa hidratação, podem ocorrer constipação intestinal, aumento de celulite, problemas renais, pele e cabelos ressecados e desidratados. Para aumentar a hidratação, é necessário obrigar-se a beber água. Um bom parâmetro para verificar maior necessidade de líquido é a cor da urina (quanto mais escura, maior a necessidade de água)”.
+CUIDADOS: </t>
+  </si>
+  <si>
+    <t>https://cdd.org.br/noticias/saiba-como-a-alimentacao-influencia-nas-dermatites/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM QUEDA DE CABELO
+INDICAÇÕES:
+A alimentação impacta diretamente na qualidade e na aparência dos cabelos. Os alimentos consumidos influenciam na força, no crescimento e na vitalidade dos fios, tornando uma dieta equilibrada e rica em nutrientes essencial para manter a saúde capilar. Segundo a dermatologista associada à Sociedade Brasileira de Dermatologia – Secção RS (SBD-RS), Ana Paula Caramori, dietas deficientes em nutrientes essenciais podem causar queda capilar.
+“A perda de cabelo pode estar relacionada a diversas causas, como doenças agudas e infecciosas, alterações hormonais, estresse ou falta de vitaminas e minerais, como ferro. Por isso, uma alimentação balanceada é fundamental para a saúde do organismo e dos nossos cabelos. Dietas pobres em proteínas e nutrientes tendem a gerar fios mais fracos e quebradiços”, afirma.
+A dermatologista destaca a importância do consumo de alimentos ricos em proteínas, aminoácidos, minerais, biotina, além de certos tipos de óleos e antioxidantes, que atuam na formação e qualidade da haste capilar.
+“Podemos citar peixes como salmão, arenque, sardinha e atum, excelentes fontes de ômega 3, que têm ação anti-inflamatória, ovos, que são uma importante fonte de proteínas e biotina, dois nutrientes fundamentais para estimular a produção de queratina, uma proteína que protege e reveste os nossos fios, vegetais de folhas verdes escuras como espinafre, couve e rúcula, ricos em nutrientes como vitaminas A e C, ferro, betacaroteno, ácido fólico e biotina, que estimulam a produção de proteínas essenciais para o fio”, destaca.
+Além disso, Ana Paula recomenda o consumo de outros alimentos, como frutas cítricas, nozes e castanha-do-pará.
+“As frutas cítricas são excelentes fontes de antioxidantes, incluindo a vitamina C. Consumir nozes, castanha-do-pará, sementes de linhaça ou de chia também é importante, pois são alimentos ricos em nutrientes que previnem a queda de cabelo, como zinco, magnésio, vitaminas do complexo B, vitamina E, selênio e ômega 3. É fundamental lembrar que o caminho está no equilíbrio, pois o excesso de selênio e vitamina A pode também causar queda de cabelo. Então, não exagere na quantidade de castanhas”, pontua.
+A dermatologista também sugere o consumo de alimentos ricos em vitamina A, como fígado, gema de ovo, óleos de peixes, cenoura, espinafre, manga, mamão, batata-doce e laticínios, além de abacate, devido à sua alta concentração de ácidos graxos essenciais e vitaminas B e E, que protegem e fortalecem o cabelo, e alecrim, uma planta medicinal rica em flavonoides, terpenos e ácidos fenólicos com propriedades antioxidantes.
+Sobre erros alimentares que prejudicam a qualidade dos fios, Ana Paula afirma que dietas muito restritivas e com baixo consumo de nutrientes podem comprometer a saúde capilar.
+“O cabelo é formado em sua maior parte por proteínas, como a queratina, que pode perder suas características estruturais em situações de carência nutricional. Portanto, dietas muito restritivas, que levem à perda de peso muito rápida ou que contenham baixo consumo de proteínas e aminoácidos, podem causar queda de cabelo e alterações importantes nos fios”, relata.
+A especialista enfatiza que a suplementação só deve ser iniciada com a orientação de um dermatologista, após uma avaliação detalhada dos cabelos e a realização de exames de sangue, recomendando evitar a automedicação.
+</t>
+  </si>
+  <si>
+    <t>https://sbdrs.org.br/saiba-quais-alimentos-ajudam-a-garantir-a-saude-dos-cabelos/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A ACNE
+Esse dano à pele do rosto, nem sempre está relacionado à alterações hormonais, comuns durante a gestação ou no período menstrual ou decorrente da utilização de produtos cosméticos como a maquiagem.
+A má alimentação é um fator contribuinte para o agravamento desse problema.
+INDICAÇÕES:
+O indicado é retirar do cardápio os nutrientes que agravam o quadro clínico.
+“Alimentos com alto índice glicêmicos são os mais prejudiciais à aparência da pele. Ao ingerir em excesso doces, tortas, balas e bolos o indivíduo estará contribuindo para a elevação dos níveis de açúcares no sangue. Tais alimentos são pobres em fibras e nutrientes e podem provocar rugas e flacidez na pele”, explica a nutricionista da Global Nutrição, Dra. Ana Huggler.
+O leite e seus derivados também são vilões da cútis, pois possuem hormônios em sua composição, contribuindo para o aumento da produção de sebo nas glândulas da pele. “Uma alimentação saudável no dia a dia é benéfica ao organismo, pois combate os radicais livres que aceleram o envelhecimento cutâneo, ajuda na restauração da pele exposta à fatores ambientais e contribui para a produção e renovação de colágeno (responsável pela sustentação da pele)”, descreve a nutricionista.
+Alguns alimentos que ajudam a prevenir o aparecimento de cravos e espinhas na derme:
+Peixes: Ricos em Ômega 3 (gordura encontrada em espécies como atum e sardinha), contém muitos nutrientes e são mais benéficos à saúde, sendo contribuidores para a redução de doenças cardíacas, nível de colesterol ruim (LDL) no sangue e triglicerídeos. Por possuírem grandes quantidades de minerais em sua composição, os peixes têm ação anti-inflamatória que ajuda na diminuição de acne.
+Frutas e verduras de cor amarela: São ricas em substâncias que ajudam a manter a pele sempre rejuvenescida e limpa. O betacaroteno encontrado em sua composição atua combatendo os processos inflamatórios. Além disso, são ricos em vitaminas A e do complexo B, fósforo, cálcio e potássio que atuam como antioxidantes do corpo. São elas: pera, banana, melão amarelo, abóbora, cenoura, damasco, laranja, pêssego, entre outros.
+Água: Fundamental para hidratação do corpo, a ingestão de dois litros de água por dia ajuda a eliminar toxinas e impurezas presentes no organismo. Além disso, o líquido deixa a pele mais viçosa e rejuvenescida, contribuindo para a formação e renovação de colágeno na pele, pois eles dependem de água para um bom funcionamento.
+</t>
+  </si>
+  <si>
+    <t>https://www.asbran.org.br/noticias/1096/muitos-alimentos-podem-ajudar-no-tratamento-para-combater-a-acne</t>
+  </si>
+  <si>
+    <t>ALIMENTOS PARA AJUDAR COM A AZIA
+A azia é causada pelo conteúdo ácido do estômago que sobe para o esôfago, que é muito menos resistente ao ácido.
+INDICAÇÕES:
+Alguns alimentos também estão associados à azia, como:
+Cebolas
+Frutas cítricas
+Alimentos à base de tomate
+Hortelã-pimenta
+Opções de alimentos com baixo teor de gordura são úteis para prenevir muitas doenças digestivas, assim como bebidas não alcoólicas.Bebidas descafeinadas são úteis para alguns pacientes, assim como um controle razoável das porções.
+Moderação tanto na alimentação quanto no consumo de álcool, e aproveitar a variedade de pratos disponíveis, é uma estratégia melhor do que medicamentos adicionais.
+Faça a refeição principal no meio do dia. Não coma nas três horas que antecedem a hora de dormir. Evite alimentos gordurosos. Beba álcool com moderação e considere elevar a cabeceira da cama.
+CUIDADOS: Se a azia vier acompanhada de outros sintomas, como vômito com sangue, alteração nas fezes, sensação de peito apertado, tosse e falta de ar, procure atendimento médico imediato.</t>
+  </si>
+  <si>
+    <t>https://www.hospitaloswaldocruz.org.br/centro-especializado/aparelho-digestivo/refluxo-gastroesofagico-azia/
+https://www.mayoclinichealthcare.co.uk/news/tips-on-eating-to-prevent-heartburn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A FALTA DE APETITE
+INDICAÇÕES:
+Procure fazer pequenas refeições e lanches frequentes, por exemplo, a cada duas horas.
+Seja positivo em relação ao que você come – cada garfada a mais ajuda.
+Tente não perder o hábito de comer – na verdade, você precisa comer para estimular o apetite.
+Seu apetite pode ir e vir, por isso é importante aproveitar ao máximo os momentos em que você sentir vontade de comer.
+Não se preocupe se não forem alimentos 'normais' em horários 'normais'.
+Tente relaxar e apreciar a sua refeição. Coma devagar e mastigue bem os alimentos, tentando descansar antes e depois.
+Evite se empanturrar com grandes porções de saladas, água e refrigerantes. Eles fornecem volume, mas pouco nutriente.
+Para aguçar o apetite, torne os alimentos visualmente atraentes: sirva pequenas porções em pratos pequenos e experimente adicionar guarnições como limão ou salsa.
+Experimente com alimentos diferentes. Você pode descobrir que gosta de coisas que normalmente não come.
+Uma breve caminhada antes das refeições ou um pouco de ar fresco podem ajudar a melhorar o apetite.
+Um pequeno copo de vinho, cerveja, xerez ou sua bebida favorita, tomado meia hora antes da refeição, pode estimular o apetite, mas consulte seu médico primeiro.
+Aceite ofertas de familiares e amigos para ajudar com as tarefas de cozinhar e fazer compras.
+Alimentos prontos para consumo são uma opção útil e podem ser igualmente nutritivos.
+Se você tiver um congelador, tente preparar a comida com antecedência quando tiver vontade de cozinhar e guarde-a para quando não estiver se sentindo bem.
+Às vezes, o cheiro da comida pode ser apetitoso, enquanto outras vezes pode ser desagradável. Se isso acontecer, tente ficar longe da cozinha enquanto a comida estiver sendo preparada (se possível) ou coma alimentos frios, que geralmente têm menos cheiro.
+</t>
+  </si>
+  <si>
+    <t>https://www.theaat.org.uk/tips-for-when-you-have-a-poor-appetite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM DORES ARTICULARES
+INDICAÇÕES:
+Um dos itens que não podem faltar no prato de quem sofre de dor crônica é o triptofano, aminoácido responsável pela síntese de serotonina. Ele é encontrado em alimentos como carnes magras, leite desnatado e banana.
+Outro elemento importante nesse processo é o carboidrato. É recomendável que 50% a 60% da ingestão calórica diária seja composta por carboidratos, presentes nas frutas, pães, batata e cereais, de preferência os integrais. O açúcar pode até provocar uma sensação imediata de energia, mas o pico nos níveis de glicose no sangue depois leva à sensação de fadiga e moleza.
+É recomendada a ingestão de alimentos ricos em magnésio (como espinafre, soja, caju, aveia e tomate), ácido fólico (laranja, maçã e folhas verdes), cálcio (leite, iogurte e queijos magros) e selênio (castanhas, nozes, atum e semente de girassol).
+Vale lembrar que o efeito desses nutrientes não é imediato e a alimentação é apenas um dos pilares do tratamento. No caso de quem sofre de fibromialgia, comer adequadamente ainda é útil para combater o excesso de peso.
+</t>
+  </si>
+  <si>
+    <t>https://www.sbcm.org.br/v2/index.php/not%C3%ADcias/1091-sp-1841400569</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM DISTÚRBIOS HEPÁTICOS
+O fígado atua como um processador de nutrientes, e algum dano no órgão pode comprometer a sua estrutura, levando a um quadro clínico de doença hepática. Estas compreendem a cirrose, a hepatite e a insuficiência hepática, sendo a cirrose a forma mais grave da doença.
+INDICAÇÕES:
+Medidas para tratamento das doenças hepáticas incluem controle da ingestão do álcool, redução do peso, controle da ingestão de gorduras e açúcares. Os alimentos benéficos para o tratamento são: chá verde ou preto, alecrim, alho, frutas cítricas e vermelhas, peixes, cereais integrais como aveia e linhaça, castanhas e leguminosas como feijão, lentilha e grão de bico. Alguns vegetais também contribuem no tratamento; Por exemplo: agrião, brócolis, couve-chinesa, couve-flor, mostarda, nabo, rabanete e repolho.
+Se você deseja um fígado saudável, a melhor estratégia é consumir alimentos de cores variadas e evitar alimentos processados, álcool e bebidas açucaradas.
+Faça pequenas refeições regulares. Não pule refeições nem coma em excesso.
+Beba de 6 a 8 copos de líquidos (de preferência água) por dia.
+Escolha regularmente uma variedade de alimentos integrais, incluindo frutas e vegetais, fontes de proteína (leguminosas, carnes magras), grãos integrais (quinoa, arroz selvagem), laticínios (iogurte com baixo teor de gordura, leite e queijo) e fontes de gordura saudável (nozes, abacate, peixes gordos).
+Consuma mais frutas e verduras frescas, especialmente as de cores vibrantes e pigmentos intensos, como laranja, amarelo, vermelho e verde.
+Lave frutas e verduras imediatamente antes de usar para remover pesticidas. Evite lavá-las com muita antecedência para reduzir a transpiração ou a deterioração.
+Ao cozinhar legumes e frutas, cozinhe-os no vapor ou asse-os. Isso preserva mais nutrientes do que fervê-los.
+Limite o consumo de gorduras saturadas e açúcar, como bebidas açucaradas, batatas fritas, bolos e comidas para viagem.
+Escolha produtos integrais em vez de produtos brancos/branqueados/refinados.
+</t>
+  </si>
+  <si>
+    <t>https://liver.org.au/living-well/eating-for-your-liver/
+https://prefeitura.sp.gov.br/web/saude/w/noticias/191060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM ÚLCERAS E GASTRITES
+A gastrite consiste na inflamação da mucosa gástrica. Pode ser desencadeada por medicamentos, ingestão de bebidas alcoólicas, fumo e situações de estresse. A úlcera é caracterizada por perda de tecido nas áreas do tubo digestório que entram em contato com a secreção ácida do estômago decorrente do desequilíbrio entre fatores que agridem a mucosa e que a protegem.
+INDICAÇÕES:
+Recomendações gerais:
+Faça as refeições em ambiente tranquilo, comendo bem devagar e mastigando bem os alimentos;
+Os alimentos devem ser ingeridos em pequenas quantidades, fracionadas, aproximadamente, de 3 em 3 horas, ou seja, de 5 a 6  refeições por dia. Evitar períodos longos em jejum;
+Mantenha um adequado consumo de líquidos: 2000ml/dia. Os líquidos auxiliam no bom funcionamento do intestino;
+O leite não deve ser consumido como um mecanismo de aliviar a dor e a queimação, pois ele estimula a produção de ácido gástrico o que poderá intensificar a dor. Deve ser utilizado como forma integrante da alimentação;
+Não fumar;
+Evite frituras, prefira os alimentos cozidos, assados e grelhados;
+O álcool é um potente irritante da mucosa gástrica que deve ser evitado;
+Respeite sua tolerância aos alimentos;
+Procure não ingerir líquidos durante as refeições, de preferência ½ hora antes ou depois.
+Alimentos que devem ser Evitados:
+Frituras;
+Café, chá mate e preto, refrigerantes, bebidas alcoólicas ou gasosas;
+Frutas ácidas como: laranja, maracujá, abacaxi e limão.
+Pimenta, mostarda, catchup, molho Inglês, extrato de tomate, conservas em geral, orégano e Coentro;
+Maionese ou Molhos Prontos;
+Alimentos enlatados e embutidos: salame, salsicha, presunto e carnes gordurosas;
+Creme de Leite, manteiga, queijos gordurosos (amarelos);
+Grãos em excesso (Feijão, Lentilha, Ervilha, Etc.)  - são recomendados o consumo de uma vez por dia;
+Chocolate e doces concentrados;
+Pimenta vermelha, malagueta, pimenta preta e condimentos picantes;
+Croissant, sonhos, folhados e produtos doces ricos em gordura.
+Alimentos que são permitidos:
+Ricos em fibras (vegetais);
+Arroz, massas sem molhos industrializados "concentrados'; 
+Legumes e verduras;
+Ovos cozidos;
+Carne bovina magra, de frango ou peixe (bem cozidos, assados ou grelhados);
+Sobremesas, exemplos: gelatinas, pudim sem calda, sagu, curau, moderadamente;
+Temperos: óleos vegetais, margarina, sal, cebola, tomate, cheiro verde;
+Chá de ervas;
+Geléia, mel, margarina ligth em quantidades moderadas;
+Leite e iogurte desnatado e queijo branco.
+</t>
+  </si>
+  <si>
+    <t>https://www.h9j.com.br/blog/dieta-para-gastrite-e-ulcera/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM OS GASES
+INDICAÇÕES:
+Seu médico pode sugerir mudanças em seus hábitos alimentares e de ingestão de bebidas para reduzir os sintomas de gases. Por exemplo, os médicos podem recomendar
+Evite ou limite a frequência com que você masca chiclete, chupa balas duras, bebe refrigerantes e usa canudo para beber.
+Evite falar enquanto come ou bebe.
+Coma devagar e, quando possível, sente-se para comer em vez de comer correndo.
+Comer porções menores e mais frequentes em vez de refeições maiores.
+Mudar sua dieta
+Algumas pessoas apresentam mais sintomas de gases quando consomem certos carboidratos  que o estômago  e o intestino delgado  não digerem completamente . Quando esses carboidratos chegam ao intestino grosso , as bactérias  os decompõem, produzindo gases nesse processo.
+Exemplos de alimentos e bebidas que contêm carboidratos e podem causar excesso de gases incluem:
+certas frutas — incluindo maçãs, pêssegos e peras — e sucos de frutas
+Vegetais, especialmente os crucíferos — um grupo que inclui brócolis, couve-flor, couve, couve-galega e outros — e leguminosas — um grupo que inclui feijões, ervilhas e lentilhas .
+Produtos lácteos, como leite, sorvete e iogurte.
+grãos integrais, como o trigo integral
+Bebidas que contêm xarope de milho rico em frutose , como sucos de frutas, refrigerantes, bebidas esportivas e bebidas energéticas.
+Doces, gomas de mascar ou outros produtos que contenham adoçantes terminados em “-ol”, como sorbitol, manitol, xilitol, eritritol e maltitol.
+Algumas pessoas apresentam mais sintomas de gases quando consomem muita fibra . Outras podem apresentar mais sintomas de gases quando consomem alimentos ricos em gordura , o que pode aumentar o inchaço .
+Converse com seu médico sobre sua dieta. Ele pode pedir que você mantenha um diário alimentar, anotando o que come e bebe e seus sintomas de gases. Esse diário pode ajudar seu médico ou nutricionista a identificar se certos alimentos e bebidas podem estar causando seus sintomas.
+</t>
+  </si>
+  <si>
+    <t>https://www.niddk.nih.gov/health-information/digestive-diseases/gas-digestive-tract/eating-diet-nutrition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A TOSSE
+INDICAÇÕES:
+Receitas para aliviar a tosse e o resfriado:
+1. Água morna com mel e limão 
+mel com água de limão
+Uma bebida quente feita com mel e limão pode ajudar a aliviar a dor de garganta e os sintomas da tosse de forma natural. O mel reveste a garganta, alivia a irritação e reduz a tosse. O limão, rico em vitamina C, fortalece o sistema imunológico e ajuda a combater os sintomas do resfriado. 
+Ingredientes: 
+1 xícara de água morna 
+1 colher de sopa de mel 
+O suco de meio limão 
+Instruções: 
+Misture o mel e o suco de limão em água morna até obter uma mistura homogênea. Beba essa bebida calmante aos poucos para aliviar a tosse e acalmar a garganta. 
+2. Chá de Gengibre e Cúrcuma
+chá de gengibre e cúrcuma
+Este chá combina dois ingredientes poderosos que fortalecem o sistema imunológico: gengibre e cúrcuma. O gengibre, com suas propriedades anti-inflamatórias, pode ajudar a aliviar a garganta e reduzir a tosse. A cúrcuma contém curcumina, um composto conhecido por seus efeitos imunomoduladores e anti-inflamatórios, que pode auxiliar no alívio dos sintomas de resfriado. 
+Ingredientes: 
+1 xícara de água 
+Um pedaço de gengibre fresco de 2,5 cm (1 polegada), descascado e ralado. 
+1/2 colher de chá de açafrão em pó 
+1 colher de sopa de mel (opcional) 
+Instruções: 
+Ferva água em uma panela e adicione gengibre ralado e açafrão em pó. Deixe em infusão por 5 minutos. Coe o chá em uma xícara. Adicione mel, se desejar, e mexa bem. Aproveite este chá que fortalece o sistema imunológico para aliviar os sintomas de tosse e resfriado. Mas lembre-se sempre de não exagerar na quantidade, pois pode ser muito quente para algumas pessoas. 
+3. Sopa de Frango com Alho 
+sopa de frango com alho
+O alho é conhecido por suas propriedades antibacterianas e antivirais, que podem ajudar a combater infecções que causam tosse e resfriado. A canja de galinha com alho combina as propriedades imunológicas do alho e da galinha, oferecendo hidratação, aconchego e nutrição provenientes dos legumes e da galinha, além de proporcionar conforto e fortalecer o sistema imunológico durante doenças. 
+Ingredientes: 
+1 colher de sopa de azeite 
+3 dentes de alho picados 
+1 cebola pequena picada 
+2 cenouras, fatiadas 
+2 talos de aipo, fatiados 
+4 xícaras de caldo de galinha 
+1 xícara de frango cozido e desfiado 
+Sal e pimenta a gosto 
+Instruções: 
+Aqueça um pouco de azeite em uma panela em fogo médio e refogue alho picado, cebola picada, cenoura e aipo. Refogue até que os legumes estejam macios. Adicione o caldo de galinha e deixe ferver. Abaixe o fogo e cozinhe em fogo brando por 15 a 20 minutos. Adicione o frango cozido e tempere com sal e pimenta. Cozinhe por mais 5 minutos. Desfrute desta sopa reconfortante e nutritiva por seus efeitos calmantes nos sintomas de tosse e resfriado. 
+Leia também: 11 benefícios incríveis da água de coco para a saúde
+4. Leite Dourado com Cúrcuma
+leite dourado de cúrcuma
+O leite dourado combina os benefícios da cúrcuma com o leite morno. A curcumina, principal composto da cúrcuma, possui propriedades anti-inflamatórias que podem aliviar a irritação das vias aéreas e suprimir a tosse. O leite morno proporciona conforto e hidratação, ajudando a aliviar os sintomas da gripe e do resfriado. 
+Ingredientes: 
+1 xícara de leite (de origem animal ou vegetal) 
+1/2 colher de chá de açafrão em pó 
+1/4 de colher de chá de canela em pó 
+1/4 de colher de chá de gengibre em pó 
+1 colher de sopa de mel (opcional) 
+Instruções: 
+Aqueça o leite em uma panela em fogo médio. Adicione a cúrcuma, a canela e o gengibre em pó. Misture bem. Aqueça até ficar morno, mas sem ferver. Se desejar, adicione o mel e mexa até dissolver. O leite dourado é conhecido por suas propriedades anti-inflamatórias e pode ajudar a aliviar os sintomas de tosse e resfriado. 
+5. Smoothie de banana com frutas vermelhas 
+smoothie de banana com frutas vermelhas
+Este smoothie rico em vitaminas combina os benefícios da banana madura com uma mistura de frutos silvestres. As bananas são ricas em vitamina C, B6 e potássio, que ajudam a fortalecer o sistema imunológico. Os frutos silvestres, como morangos e mirtilos, são frutas ricas em antioxidantes e com alto teor de vitamina C, que podem aliviar a tosse e fortalecer o sistema imunológico. 
+Ingredientes: 
+1 banana madura 
+1/2 xícara de frutas vermelhas misturadas (como morangos, mirtilos ou framboesas) 
+1 xícara de leite de amêndoa ou qualquer outra alternativa de leite de sua preferência. 
+1 colher de sopa de mel (opcional) 
+Cubos de gelo (opcional) 
+Instruções: 
+Bata todos os ingredientes no liquidificador até obter uma mistura homogênea. Se preferir mais gelado, adicione alguns cubos de gelo. Este smoothie rico em nutrientes fortalece o sistema imunológico durante resfriados e tosses. 
+CUIDADOS: </t>
+  </si>
+  <si>
+    <t>https://pharmeasy.in/blog/12-best-foods-to-ease-your-cough-and-cold/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A CONGESTÃO NASAL
+INDICAÇÕES:
+Top 3 alimentos para aliviar congestão nasal:
+Alho e cebola:
+Esses temperos não apenas adicionam sabor às refeições, mas também combatem infecções por bactérias, vírus e fungos. O componente alicina presente ajuda a diluir o muco, bloqueia as vias respiratórias e reduz a inflamação nasal, proporcionando alívio.
+Canja de galinha:
+A canja de galinha contém o aminoácido cisteína, que age como anti-inflamatório, acelerando a fluidificação do muco e aliviando a congestão nasal. Além disso, o vapor da sopa, juntamente com as altas temperaturas, aquece e umidifica a mucosa nasal, promovendo uma resposta fisiológica que resulta no descongestionamento do nariz.
+Gengibre:
+O consumo de gengibre é eficaz para reduzir sintomas de congestionamento, graças às suas propriedades descongestionantes que limpam as vias respiratórias. O gengibre também contém substâncias anti-inflamatórias, tornando-se um aliado no combate a gripes e resfriados, aliviando a congestão nasal associada a esses problemas de saúde.
+A escolha adequada de alimentos pode contribuir para aliviar a congestão nasal, enquanto é crucial evitar ou consumir com moderação aqueles que agravam o sintoma, causando vasodilatação, aumento da produção de muco e piora nos sintomas respiratórios. Conhecer esses alimentos pode ser fundamental para um alívio eficaz.
+</t>
+  </si>
+  <si>
+    <t>https://minhasaude.proteste.org.br/3-alimentos-que-podem-aliviar-os-sintomas-da-congestao-nasal/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR NA LACTAÇÃO
+INDICAÇÕES:
+O que se deve comer e evitar na fase de amamentação?
+Sucos de frutas naturais
+O leite materno é composto em 80% por água, por isso é muito importante que a mulher beba muita água e se mantenha sempre hidratada. Uma das formas de repor os líquidos de maneira saudável e saborosa é optando pelos sucos de frutas. Escolha frutas ricas em água, como melancia e melão, por exemplo. Porém, um alerta: cuidado com o excesso! Você pode acabar ingerindo muitas calorias de uma só vez.
+Água de coco
+Outra forma de se manter hidratada na fase de amamentação é ingerindo água de coco. Além de ajudar a estimular a produção de leite materno, ela traz muitos benefícios e nutrientes como sódio e potássio, que ajudam a equilibrar os líquidos do corpo.
+Sopa de legumes
+É essencial que a mãe lactante cuide bem de sua alimentação, consumindo sempre muitos vegetais. Para quem busca uma forma prática de consumir nutrientes, as sopas de legumes são uma ótima opção. Elas contém bastante líquido e ajudam o corpo a metabolizar o leite materno com mais facilidade.
+Alimentos integrais
+Alimentos ricos em fibras, como os cereais integrais, são fontes de bons carboidratos que vão garantir energia para a mãe e, através disso, colaboram para a produção de leite. Eles também estimulam o funcionamento do intestino e melhoram a digestão.
+Alimentos ricos em ferro
+Alimentos ricos em ferro são essenciais para quem está amamentando, pois o nutriente estimula a produção de hemoglobinas, que baixam significativamente depois do parto. Além disso, esses alimentos são importantes para saúde do bebê, pois previnem a anemia infantil. O ferro pode ser encontrado em alimentos como carnes magras, feijões e folhas verdes.
+CUIDADOS: 
+O que deve não se deve comer durante a amamentação?
+Alimentos ultraprocessados
+As mamães devem evitar alimentos industrializados e ultraprocessados como enlatados, embutidos, refrigerantes, biscoitos e sorvetes. Esses alimentos são pobres de nutrientes, cheios de açúcares e gorduras saturadas. Desse modo, acabam atrapalhando a produção de leite.
+Álcool
+Mulheres em fase de amamentação não devem consumir álcool, já que ele é rapidamente metabolizado e absorvido pelo leite materno. esse modo, faz com que o leite tenha a mesma concentração de álcool que foi ingerida pela mãe. Com isso, o bebê também acaba consumindo a substância, mas não pode metabolizá-la. Além disso, o álcool desidrata a mãe, atrapalhando a produção de leite.
+Alimentos ricos em cafeína
+Alimentos ricos em cafeína como café, chá-verde e preto, refrigerantes de cola e energéticos devem ser evitados. Isso é recomendado porque a cafeína é um estimulante e pode atrapalhar o sono do bebê, deixando-o mais irritado. O ideal é tomar no máximo 2 xícaras de café por dia ou optar pelo café descafeinado.
+</t>
+  </si>
+  <si>
+    <t>https://minhasaude.proteste.org.br/o-que-as-maes-devem-comer-na-fase-da-amamentacao/?gad_source=1&amp;gad_campaignid=22453012222&amp;gbraid=0AAAAAC-dlZxRVw-vQpJNCfQ_L3EMaTGRB&amp;gclid=CjwKCAiAuIDJBhBoEiwAxhgyFvvKSVxG8I9-ctlzXC8oPD28VC6fr5I3NEJ_5KXdXi-QzpRTIvVT6xoC44EQAvD_BwE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM OS ENJOOS
+INDICAÇÕES:
+Dê preferência aos alimentos mais secos, como torradas, pães, bolachas e biscoito (sem recheios). A consistência desse tipo de alimento auxilia no controle da sialorreia (aumento da produção de saliva), um dos sintomas comuns durante a náusea. Outro fator importante é que, por serem fontes de carboidratos, são de fácil mastigação, digestão e absorção, contribuindo com o controle da taxa de açúcar no sangue (glicemia). Também apresentam sabor neutro, o que diminui o estímulo sensorial do reflexo do vômito.
+Banana nanica é um ótimo aliado para ajudar a controlar o enjoo, além de ser um alimento com consistência mole, o que torna a digestão mais fácil e reduz a possibilidade de contração do estômago, que pode causar o vômito. A fruta também é rica em potássio, que controla o vômito, e vitamina B, que ajuda a evitar a náusea.
+Procure consumir raspadinha de gelo ou mesmo um cubo de gelo 40 minutos antes das refeições. Inclusive, se possível opte pelas preparações em temperatura ambiente ou por ingerir alimentos frios. A baixa temperatura amortece os receptores de paladar, o que pode ajudar na deglutição do alimento.
+Frutas cítricas (como limão, por exemplo), são ricas em ácido fólico, uma vitamina do complexo B que estimula a formação dos ácidos digestivos, favorecendo o esvaziamento gástrico e diminuindo o surgimento de enjoos. Alguns pacientes reduzem muito a sensação de náusea ao chupar sorvete de limão ou mesmo a fruta in natura.
+Deve-se priorizar a ingestão de oito a dez copos de líquidos entre as refeições para evitar desidratação. Essa medida minimiza a pressão no estômago, reduzindo a ocorrência de refluxo. Entre os líquidos, boas opções são os líquidos claros, como sucos, chás e caldos, limitando o uso de líquidos com muita cafeína, incluindo refrigerantes à base de cola, café e chá preto ou mate ou verde.
+</t>
+  </si>
+  <si>
+    <t>https://vencerocancer.org.br/cinco-alimentos-que-ajudam-controlar-o-enjoo/?gad_source=1&amp;gad_campaignid=22596549316&amp;gbraid=0AAAAADPLv-ow5J64au8patm-hAW46rd9H&amp;gclid=CjwKCAiAuIDJBhBoEiwAxhgyFrrAayH9g7dzSDEnJu5uzFEmPwGKC1P7-TnT5JnnV3Z5wC6R0ADAQRoClh8QAvD_BwE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A DIARRÉIA
+INDICAÇÕES:
+- A dieta BRAT
+"BRAT" não significa salsicha bratwurst neste caso. (Lembre-se, estamos falando de comidas simples, o que definitivamente exclui essa iguaria típica de churrascos.)
+A dieta BRAT é uma sigla que significa:
+Bananas . O amido presente na fruta ajuda a absorver água no cólon, o que contribui para firmar as fezes. Além disso, é rica em potássio, um eletrólito essencial que você perde com a diarreia.
+Arroz . Nesse caso, prefira o arroz branco ao arroz integral , pois é mais fácil de digerir.
+Purê de maçã . Procure comprar purê de maçã sem açúcar para reduzir o consumo de açúcar.
+Torrada . Tente usar pão branco, que é mais fácil de digerir, em vez de pão integral.
+Do ponto de vista nutricional, a dieta BRAT não é a melhor opção. Ela é pobre em proteínas, fibras e muitas vitaminas. Mas o objetivo da dieta BRAT não é atender a todos os requisitos nutricionais. Em vez disso, é uma maneira rápida e eficaz de firmar as fezes.
+Portanto, considere isso uma solução temporária para usar por um ou dois dias.
+- Alimentos insossos
+Se você deseja complementar a dieta BRAT, os seguintes alimentos podem trazer um pouco de variedade, além de serem suaves para o estômago:
+Aveia.
+Cereal seco.
+Batatas cozidas ou assadas (descascadas).
+Frango assado sem pele.
+- Bebidas eletrolíticas
+A diarreia geralmente não é um problema que se resolve apenas uma vez. Idas frequentes ao banheiro por causa da diarreia podem levar a uma perda significativa de líquidos ao longo do dia — e isso pode causar desidratação rapidamente .
+Repor os fluidos e nutrientes internos do corpo é essencial para evitar a desidratação e suas complicações. A solução? Experimente bebericar bebidas ricas em eletrólitos (como Gatorade® ou Pedialyte®).
+Bebidas eletrolíticas oferecem uma vantagem adicional devido à quantidade de sódio e açúcar em sua composição. O sódio retarda a perda de líquidos e ajuda na retenção hídrica. O açúcar, por sua vez, auxilia o organismo na absorção do sódio. Uma situação vantajosa para todos!
+- Alimentos salgados
+O sal contém sódio, que — como mencionamos acima — ajuda a manter os níveis de fluidos. Comer biscoitos de água e sal ou pretzels pode fornecer um rápido aporte de sódio, além de ser suave para o estômago.
+E sempre tem a canja de galinha, o clássico prato para quando se está doente, que geralmente contém uma boa quantidade de sódio. (Bônus adicional: o caldo de galinha pode ajudar a prevenir a desidratação.)
+Em geral, não recomendamos o consumo excessivo de sal ou sódio, mas quando se tem uma diarreia significativa, é importante garantir a ingestão suficiente para evitar uma visita ao pronto-socorro.
+- Probióticos
+Consumir alimentos com probióticos pode ajudar o intestino a se recuperar de uma infecção diarreica. As bactérias vivas presentes nos probióticos ajudam a restaurar as bactérias intestinais benéficas necessárias para manter um microbioma intestinal saudável .
+Iogurte ou kefir, uma bebida láctea fermentada, seriam boas opções, apesar de serem produtos lácteos, que geralmente são contraindicados em casos de diarreia, afirma o Dr. Kirby. (Apenas certifique-se de que o iogurte ou o kefir tenham baixo teor de açúcar.)
+</t>
+  </si>
+  <si>
+    <t>https://health.clevelandclinic.org/what-to-eat-when-you-have-diarrhea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A ANSIEDADE
+Uma alimentação saudável e equilibrada ajuda a aplacar os efeitos nocivos da ansiedade sobre a saúde. Alguns alimentos, como a alface, o farelo de aveia e o abacate, atuam no combate ao estresse, favorecem o sono e fornecem a matéria-prima de que o organismo precisa para fabricar neurotransmissores -- substâncias químicas que regulam o humor e induzem ao relaxamento, provocando sensação de bem-estar. Confira abaixo algumas das melhores fontes de nutrientes para quem quer sair do estado de agitação mental.
+INDICAÇÕES:
+Maracujá
+Essa é receita da vovó, mas realmente funciona. A fruta é considerada um sedativo natural, graças à presença de passiflora em sua composição. Para garantir um dia mais calmo, a orientação é beber duas xícaras (chá) de suco concentrado, uma de manhã e outra à tarde. Só não exagere. "Se tomar mais do que três xícaras, há risco de ter sonolência", afirma a nutricionista Samanta Brito.
+Chá de camomila
+Possui substâncias como lactonas e alfa bisabolol, que têm efeito calmante. Pode ser consumido diariamente, de preferência, antes de dormir. Uma xícara é o suficiente para induzir a um sono mais profundo.
+Alface
+A substância que dá à folha a propriedade calmante é a lactucina, concentrada, principalmente, no talo. A verdura deve estar no cardápio diariamente, em quantidade equivalente a um prato (sobremesa) por refeição. Para variar, a dica é apostar em diferentes tipos de molhos e combinar a alface a outras variedades de folhas, legumes e frutas. Também é possível fazer chá das folhas de alface, priorizando o talo no preparo da infusão.
+Farelo de aveia e de trigo
+São fontes de magnésio, mineral que promove o relaxamento. Também contêm vitaminas do complexo B e fibras, que dão uma força ao funcionamento intestinal e favorecem a síntese de serotonina – neurotransmissor responsável pela sensação de bem-estar. "O complexo B, em particular, é fundamental para modular a química cerebral, que, por sua vez, regula o humor", diz a nutricionista Roseli Rossi. No dia a dia, o alimento pode ser adicionado a iogurtes, frutas, mingaus, vitaminas e shakes, na quantidade mínima de 1 colher (sopa).
+Abacate
+Além do magnésio, contém beta sitosterol, substância que atua na regulação do cortisol -- conhecido como o hormônio do estresse, que deixa o corpo todo em ritmo acelerado. Também dá uma força ao funcionamento intestinal, facilitando a síntese de neurotransmissores que melhoram o humor. Pode ser consumido diariamente, nos lanches, mas é importante não exceder a quantidade de 2 colheres (sopa). Embora tenha uma gordura saudável em sua composição, ele também tem muitas calorias.
+Frutas cítricas
+Laranja, morango e kiwi, entre outras, são ricas em ácido fólico, potássio e vitamina C, nutrientes que atuam sobre o sistema nervoso, combatendo o stress e o cansaço. Segundo os especialistas, as frutas cítricas também ajudam a diminuir a irritabilidade. Comer uma porção por dia – 1 laranja, 1 kiwi ou 10 morangos – garante que o organismo estará bem abastecido com esses nutrientes essenciais.
+Banana
+A vitamina B6 facilita a síntese de serotonina. Já o magnésio da fruta promove o relaxamento. Vale comer uma por dia, entre as refeições ou no café da manhã.
+Chocolate 60% cacau
+Não é à toa que ele é a escolha de muitas mulheres para amenizar os sintomas da TPM. A explicação está nas substâncias que contém, como a feniletilamina e o magnésio. Ambas participam da regulação dos níveis de estresse, promovem a liberação de substâncias que melhoram o humor e favorecem o bem-estar. Para que a escolha não pese na balança, dois quadradinhos pequenos, por dia, são a medida ideal.
+Nozes, amêndoas e castanhas-do-pará
+Elas fazem parte da turma de oleaginosas. São alimentos ricos em magnésio, vitaminas do complexo B e triptofano, que contribuem para minimizar o estresse, combater a depressão e ainda induzem ao sono. Porém, como contêm gordura – ainda que considerada boa --, deve ser consumida com moderação, por conta das calorias que oferecem. Em razão disso, o consumo diário deve ser de um punhado, com um mix dessas oleaginosas.
+Lentilha, grão-de-bico e ervilha
+São outras boas fontes de magnésio, mineral de importância fundamental para o bom funcionamento do sistema nervoso. Basta uma concha pequena de um desses alimentos, cozido, nas refeições principais, para ajudar a aliviar os sintomas da ansiedade. Versátil, essas leguminosas vão bem em saladas, cremes e pastas.
+</t>
+  </si>
+  <si>
+    <t>https://hospitalsiriolibanes.org.br/imprensa/alimentos-calmantes-controlam-a-ansiedade-mas-e-preciso-consumir-sempre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A ROUQUIDÃO
+INDICAÇÕES:
+Água
+A lista não poderia começar sem citar a bebida mais consumida do mundo. Ela, além de hidratar a garganta para deixar a voz bem preservada, pode ser misturada com um pouco de sal para formar um soro fisiológico que ajuda na hidratação da superfície instantaneamente.
+Frutas
+De fato, comer a maçã antes de uma apresentação tem o seu fundo de verdade. Por mais que o efeito não seja imediato, o consumo de frutas ricas em água como melancia e melão ajudam a manter a garganta hidratada. Além disso, alguns estudos sugerem que o extrato de frutas mais ácidas, como o maracujá, também tenha efeito positivo na proteção vocal.
+Gengibre
+O alimento é usado na medicina ayurvédica para ajudar a limpar a língua e a garganta. Ele ainda é rico em gingerol, substância que possui efeitos anti-inflamatórios e que pode combater infecções na laringe.
+Mel
+O alimento produzido pelas abelhas é uma rica fonte de antioxidantes, e já foi comprovado cientificamente que ele pode ajudar na melhora do tratamento de sintomas de infecção respiratória. Outros produtos, como o extrato de própolis, também são capazes de exercer uma função similar.
+</t>
+  </si>
+  <si>
+    <t>https://nutritotal.com.br/publico-geral/material/4-alimentos-que-fazem-bem-para-a-voz/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A ESTOMATITE
+Estomatite é o nome dado à inflamação da mucosa oral, localizada na boca, e pode afetar o interior das bochechas, gengivas, língua, lábios e o palato (céu da boca).
+INDICAÇÕES:
+Quando o paciente se encontra com o quadro de estomatite, o recomendado sempre é evitar frutas ácidas como laranja, limão, kiwi ou abacaxi, além de alimentos salgados. O ideal é beber líquidos frios, desde água até suco de frutas, e ingerir alimentos gelados como iogurte e gelatina, bem como alimentos pastosos como sopas e purês.
+</t>
+  </si>
+  <si>
+    <t>https://www.rededorsaoluiz.com.br/doencas/estomatite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A FARINGITE
+INDICAÇÕES:
+Enquanto alimentos calmantes e nutritivos podem ajudar a reduzir a inflamação e fortalecer o sistema imunológico, opções muito ácidas, gordurosas ou crocantes podem irritar ainda mais a mucosa da garganta.
+Durante esse período, optar por uma boa alimentação é essencial para acelerar a recuperação e evitar desconfortos ainda maiores.
+- 5 alimentos que ajudam a aliviar a garganta inflamada
+1. Mel e própolis
+O mel é uma opção bem tradicional no alívio da garganta inflamada. Ele tem propriedades antibacterianas e anti-inflamatórias, além de formar uma camada protetora que reduz a irritação. Já o própolis potencializa esses benefícios, ajudando a combater infecções.
+2. Chás mornos, como camomila e gengibre
+Chás são ótimos aliados para hidratar e acalmar a garganta. A camomila tem efeito relaxante e anti-inflamatório, enquanto o gengibre ajuda a combater infecções e aliviar dores. Mas atenção na temperatura: o ideal é consumir chás mornos e não quentes demais.
+3. Sopas e caldos quentes (não muito quentes)
+Além de serem fáceis de engolir, sopas e caldos são reconfortantes e ricos em nutrientes. Eles ajudam a manter o corpo hidratado e fornecem energia para o organismo se recuperar. Porém, assim como com os chás, cuidado com a temperatura!
+4. Frutas macias e hidratantes, como melancia e pera
+Frutas ricas em água e com textura macia são excelentes escolhas. Elas ajudam a hidratar o corpo e são suaves para a garganta, sem causar irritação.
+5. Iogurte natural e outros alimentos ricos em probióticos
+Probióticos fortalecem o sistema imunológico e ajudam o corpo a combater infecções. O iogurte natural, além de nutritivo, tem uma textura cremosa que é muito bem-vinda em um quadro de garganta inflamada.
+- 5 alimentos que podem prejudicar a garganta inflamada
+1. Alimentos muito ácidos, como laranja e abacaxi
+Embora sejam ricos em vitamina C, frutas cítricas podem causar ardência e irritar a mucosa da garganta. Nesse período, prefira outras fontes de vitamina C, como mamão ou morango.
+2. Bebidas geladas e gaseificadas
+Bebidas muito geladas podem causar choque térmico, enquanto as gaseificadas podem irritar ainda mais a garganta. O ideal nesse momento é optar por líquidos mornos ou em temperatura ambiente.
+3. Frituras e alimentos gordurosos 
+Frituras são difíceis de digerir e podem aumentar o risco de refluxo, que é um dos fatores que agravam a inflamação na garganta.
+4. Doces com alto teor de açúcar
+O que acontece é que o açúcar em excesso pode enfraquecer o sistema imunológico e favorecer o crescimento de bactérias, dificultando a recuperação.
+5. Alimentos duros ou crocantes, como torradas e biscoitos
+ Esses alimentos podem machucar a mucosa da garganta, causando ainda mais desconforto. Dê preferência a opções macias e fáceis de mastigar.
+</t>
+  </si>
+  <si>
+    <t>https://www.gndiminas.com.br/blog-da-saude/10-alimentos-pra-garganta-inflamada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM AS AFTAS
+INDICAÇÕES:
+Alimentos a evitar:
+As aftas reagem muito mal perante determinado tipo de alimentos. Para prevenir as aftas, evite ingerir:
+Alimentos picantes ou muito condimentados
+Alimentos salgados, como alguns snacks, amendoins ou batatas fritas
+Frutas cítricas ou ácidas, como laranjas, limões e morangos
+Alimentos demasiado duros, como tostas ou frutos secos
+Alimentos ou bebidas quentes (como café)
+Refrigerantes (por causa do açúcar branco)
+Chocolate
+O que deve comer para evitar as aftas:
+Como forma de prevenir e ajudar a tratar as aftas, faça uma alimentação saudável, privilegiando:
+Alimentos que forneçam a quantidade necessária de vitaminas e sais minerais
+Alimentos macios, como sopas de legumes e purés
+Bebidas frias, como água e chás
+</t>
+  </si>
+  <si>
+    <t>https://www.cuf.pt/mais-saude/aftas-qual-origem-e-que-alimentos-evitar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A DIABETES
+INDICAÇÕES:
+- vegetais folhosos verde-escuros  
+Ricas em vitaminas e minerais como as vitaminas A, C, K e folato; ferro; cálcio; e potássio, essas frutas e vegetais são pobres em calorias e carboidratos e se encaixam na seção de vegetais não amiláceos do Prato do Diabético. Além disso, experimente adicionar vegetais folhosos escuros, como espinafre, couve e couve-galega, a saladas, sopas e ensopados.
+- Abacate
+Este alimento rico em nutrientes é importante por fornecer vitaminas lipossolúveis e fibras, além de ajudar a promover a sensação de saciedade. O abacate não é apenas versátil e delicioso, como também oferece uma fonte de gordura saudável para o coração, sendo uma ótima opção para a dieta do diabético. 
+- Feijões, ervilhas secas e leguminosas
+Esses alimentos são verdadeiras estrelas das proteínas vegetais, pois são ricos em fibras, folato, potássio, ferro e zinco. Existem diferentes tipos de feijão, como o feijão-carioca, o feijão-preto, o feijão-carioca, o feijão-branco e o feijão-preto, e leguminosas como grão-de-bico, ervilha e lentilha, que oferecem uma série de benefícios nutricionais.
+Essas proteínas vegetais contêm carboidratos, mas ½ xícara fornece tanta proteína quanto 30 gramas de carne, sem a gordura saturada. Para economizar tempo, você pode usar feijão enlatado. Mas certifique-se de escorrer e enxaguar bem para remover o máximo de sal possível. Optar por feijões, ervilhas e outras leguminosas secas não só é econômico, como também permite personalizá-las com seus próprios temperos.
+- Peixes ricos em ácidos graxos ômega-3
+Os ácidos graxos ômega-3 podem ajudar a reduzir o risco de doenças cardíacas e inflamações. Peixes ricos nesses ácidos graxos saudáveis ​​são às vezes chamados de "peixes gordos". O salmão é bem conhecido nesse grupo, e outros peixes ricos em ômega-3 incluem arenque, sardinha, cavala, truta e atum albacora.
+Escolha peixes grelhados, assados ​​ou cozidos na brasa para evitar o excesso de carboidratos e calorias presentes em peixes empanados e fritos. Procure consumir peixes gordos pelo menos duas vezes por semana para obter seus benefícios nutricionais.
+O Relatório de Consenso sobre Nutrição afirma:
+“A recomendação para o público em geral de consumir uma porção de peixe (especialmente peixes gordos) pelo menos duas vezes por semana também é apropriada para pessoas com diabetes.”
+- Nozes
+Uma porção de nozes pode ser uma ótima fonte de gorduras saudáveis, magnésio e fibras, além de ajudar a controlar a fome. Algumas nozes e sementes, como nozes comuns e linhaça, também são boas fontes de ômega-3. Experimente torrar e temperar suas próprias nozes para reduzir o sódio adicionado presente nas nozes processadas.
+- Frutas vermelhas
+As frutas vermelhas são uma ótima opção para um plano alimentar para diabéticos, pois são ricas em antioxidantes, vitaminas C e K, manganês, potássio e fibras. Por serem naturalmente doces, podem ser uma excelente opção para satisfazer a vontade de doce sem adição de açúcar.
+- Frutas cítricas
+A maioria de nós sabe que as frutas cítricas são uma ótima fonte de vitamina C, mas você sabia que elas também contêm fibras, ácido fólico e potássio? De toranjas, laranjas, limões, limas e outras frutas, prefira as frutas inteiras aos sucos para obter todos os benefícios de consumi-las, incluindo as fibras da polpa.
+- Grãos integrais
+Os grãos integrais são ricos em vitaminas e minerais como vitaminas do complexo B, magnésio, ferro e manganês. Também são uma ótima fonte de fibras. Procure produtos cujo primeiro ingrediente seja a palavra "integral". Alguns exemplos de grãos integrais incluem aveia integral, quinoa, cevada, farro e trigo integral.
+- Leite e iogurte
+Você já deve ter ouvido falar que leite e iogurte ajudam a fortalecer ossos e dentes graças ao cálcio. Além do cálcio, muitos produtos lácteos e iogurtes são enriquecidos com vitamina D, o que os torna uma boa fonte desse mineral. Cada vez mais pesquisas estão sendo realizadas sobre a relação entre a vitamina D e a saúde.
+Leite e iogurte contêm carboidratos, que você precisará controlar se tiver diabetes. Procure iogurtes com baixo teor de gordura e açúcar adicionado. Experimente adicionar um pouco de adoçante natural ao iogurte grego natural desnatado com frutas vermelhas e finalize com nozes para um café da manhã delicioso.
+</t>
+  </si>
+  <si>
+    <t>https://diabetes.org/food-nutrition/food-and-blood-sugar/diabetes-superstar-foods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A DEPRESSÃO
+Quer saber quais alimentos melhoram o humor e são ótimos para dar uma forcinha no combate à depressão?
+INDICAÇÕES:
+Ovos: Eles são uma boa fonte de vitaminas do complexo B, que colaboram com o bom humor. O recomendado é uma unidade por dia, no máximo. Quem tem colesterol alto deve se preocupar com o consumo excessivo e evitar este alimento frito.
+Castanha-do-pará: É rica em selênio, um poderoso agente antioxidante. A castanha pode ajudar na redução do estresse. São recomendadas de duas a três unidades diárias.
+Nozes e amêndoas: Também são fontes ricas de selênio e ajudam a minimizar os sintomas. Recomendação é de quatro a cinco unidades de nozes ou 10 a 12 unidades de amêndoas. Também dá para fazer uma mistura dos dois sabores.
+Mel: É estimulante e ajuda na produção de serotonina, neurotransmissor responsável pela sensação de prazer e bem-estar. Para usufruir dos benefícios, duas colheres de sobremesa ao dia são suficientes.
+Leite e iogurte desnatado: São fontes ricas de cálcio, mineral que elimina a tensão e depressão. O cálcio ajuda a reduzir e controlar o nervosismo e a irritabilidade. É recomendado o consumo de 2 a 3 porções por dia.
+Melancia, abacate, mamão, banana, tangerina e limão: Todas essas frutas são ricas em triptofano, aminoácido que ajuda na produção de serotonina. É recomendado o consumo de três a cinco porções de frutas todos os dias.
+Laranja e maçã: São excelente fontes de ácido fólico, cujo consumo está associado à menor prevalência de sintomas depressivos. Além de ser rica em vitamina C, a laranja promove o melhor funcionamento do sistema nervoso, garante energia, ajuda a combater o estresse e previne a fadiga.
+CUIDADOS: </t>
+  </si>
+  <si>
+    <t>https://coren-se.gov.br/conheca-os-alimentos-que-ajudam-no-combate-a-depressao/</t>
   </si>
 </sst>
 </file>
@@ -2276,9 +3208,11 @@
         <v>92</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
-      <c r="D34" s="7"/>
+      <c r="D34" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
@@ -2305,12 +3239,14 @@
     <row r="35">
       <c r="A35" s="7"/>
       <c r="B35" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
-      <c r="D35" s="7"/>
+      <c r="D35" s="8" t="s">
+        <v>96</v>
+      </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
@@ -2337,12 +3273,14 @@
     <row r="36">
       <c r="A36" s="7"/>
       <c r="B36" s="5" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
-      <c r="D36" s="7"/>
+      <c r="D36" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -2369,12 +3307,14 @@
     <row r="37">
       <c r="A37" s="7"/>
       <c r="B37" s="5" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
-      <c r="D37" s="7"/>
+      <c r="D37" s="9" t="s">
+        <v>100</v>
+      </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -2401,10 +3341,10 @@
     <row r="38">
       <c r="A38" s="7"/>
       <c r="B38" s="5" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -2433,12 +3373,14 @@
     <row r="39">
       <c r="A39" s="7"/>
       <c r="B39" s="5" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
-      <c r="D39" s="7"/>
+      <c r="D39" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
@@ -2465,12 +3407,14 @@
     <row r="40">
       <c r="A40" s="7"/>
       <c r="B40" s="5" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
-      <c r="D40" s="7"/>
+      <c r="D40" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
@@ -2496,9 +3440,15 @@
     </row>
     <row r="41">
       <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
+      <c r="B41" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>107</v>
+      </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -2524,9 +3474,15 @@
     </row>
     <row r="42">
       <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
+      <c r="B42" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>109</v>
+      </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
@@ -2552,9 +3508,15 @@
     </row>
     <row r="43">
       <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
+      <c r="B43" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>111</v>
+      </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
@@ -2580,9 +3542,15 @@
     </row>
     <row r="44">
       <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
+      <c r="B44" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
@@ -2608,9 +3576,15 @@
     </row>
     <row r="45">
       <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
+      <c r="B45" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>115</v>
+      </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
@@ -2636,9 +3610,15 @@
     </row>
     <row r="46">
       <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
+      <c r="B46" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>117</v>
+      </c>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
@@ -2664,9 +3644,15 @@
     </row>
     <row r="47">
       <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
+      <c r="B47" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>119</v>
+      </c>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
@@ -2692,9 +3678,15 @@
     </row>
     <row r="48">
       <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
+      <c r="B48" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>121</v>
+      </c>
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
@@ -2720,9 +3712,15 @@
     </row>
     <row r="49">
       <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
+      <c r="B49" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
@@ -2748,9 +3746,15 @@
     </row>
     <row r="50">
       <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
+      <c r="B50" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>125</v>
+      </c>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
@@ -2776,9 +3780,15 @@
     </row>
     <row r="51">
       <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
+      <c r="B51" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>127</v>
+      </c>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
@@ -2804,9 +3814,15 @@
     </row>
     <row r="52">
       <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
+      <c r="B52" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
@@ -2832,9 +3848,15 @@
     </row>
     <row r="53">
       <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
+      <c r="B53" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>131</v>
+      </c>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
@@ -2860,9 +3882,15 @@
     </row>
     <row r="54">
       <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
+      <c r="B54" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>133</v>
+      </c>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
@@ -2888,9 +3916,15 @@
     </row>
     <row r="55">
       <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
+      <c r="B55" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>135</v>
+      </c>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
@@ -2916,9 +3950,15 @@
     </row>
     <row r="56">
       <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
+      <c r="B56" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
@@ -2944,9 +3984,15 @@
     </row>
     <row r="57">
       <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
+      <c r="B57" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>139</v>
+      </c>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
@@ -2972,9 +4018,15 @@
     </row>
     <row r="58">
       <c r="A58" s="7"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
+      <c r="B58" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>141</v>
+      </c>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
@@ -3000,9 +4052,15 @@
     </row>
     <row r="59">
       <c r="A59" s="7"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
+      <c r="B59" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>143</v>
+      </c>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
@@ -3028,9 +4086,15 @@
     </row>
     <row r="60">
       <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
+      <c r="B60" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>145</v>
+      </c>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
@@ -3055,10 +4119,16 @@
       <c r="Z60" s="7"/>
     </row>
     <row r="61">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>147</v>
+      </c>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
@@ -3083,10 +4153,16 @@
       <c r="Z61" s="7"/>
     </row>
     <row r="62">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
+      <c r="A62" s="5"/>
+      <c r="B62" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>149</v>
+      </c>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
@@ -3111,10 +4187,16 @@
       <c r="Z62" s="7"/>
     </row>
     <row r="63">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>151</v>
+      </c>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
@@ -3139,10 +4221,16 @@
       <c r="Z63" s="7"/>
     </row>
     <row r="64">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>153</v>
+      </c>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
@@ -3167,10 +4255,16 @@
       <c r="Z64" s="7"/>
     </row>
     <row r="65">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
+      <c r="A65" s="5"/>
+      <c r="B65" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>155</v>
+      </c>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
@@ -3195,10 +4289,16 @@
       <c r="Z65" s="7"/>
     </row>
     <row r="66">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>157</v>
+      </c>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
@@ -3223,10 +4323,16 @@
       <c r="Z66" s="7"/>
     </row>
     <row r="67">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>159</v>
+      </c>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
@@ -3251,10 +4357,16 @@
       <c r="Z67" s="7"/>
     </row>
     <row r="68">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
+      <c r="A68" s="5"/>
+      <c r="B68" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>161</v>
+      </c>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
@@ -3279,10 +4391,16 @@
       <c r="Z68" s="7"/>
     </row>
     <row r="69">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
+      <c r="A69" s="5"/>
+      <c r="B69" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>163</v>
+      </c>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
@@ -3307,10 +4425,16 @@
       <c r="Z69" s="7"/>
     </row>
     <row r="70">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
+      <c r="A70" s="5"/>
+      <c r="B70" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>165</v>
+      </c>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
@@ -3335,10 +4459,16 @@
       <c r="Z70" s="7"/>
     </row>
     <row r="71">
-      <c r="A71" s="7"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>167</v>
+      </c>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
@@ -29150,232 +30280,8 @@
       <c r="Y992" s="7"/>
       <c r="Z992" s="7"/>
     </row>
-    <row r="993">
-      <c r="A993" s="7"/>
-      <c r="B993" s="7"/>
-      <c r="C993" s="7"/>
-      <c r="D993" s="7"/>
-      <c r="E993" s="7"/>
-      <c r="F993" s="7"/>
-      <c r="G993" s="7"/>
-      <c r="H993" s="7"/>
-      <c r="I993" s="7"/>
-      <c r="J993" s="7"/>
-      <c r="K993" s="7"/>
-      <c r="L993" s="7"/>
-      <c r="M993" s="7"/>
-      <c r="N993" s="7"/>
-      <c r="O993" s="7"/>
-      <c r="P993" s="7"/>
-      <c r="Q993" s="7"/>
-      <c r="R993" s="7"/>
-      <c r="S993" s="7"/>
-      <c r="T993" s="7"/>
-      <c r="U993" s="7"/>
-      <c r="V993" s="7"/>
-      <c r="W993" s="7"/>
-      <c r="X993" s="7"/>
-      <c r="Y993" s="7"/>
-      <c r="Z993" s="7"/>
-    </row>
-    <row r="994">
-      <c r="A994" s="7"/>
-      <c r="B994" s="7"/>
-      <c r="C994" s="7"/>
-      <c r="D994" s="7"/>
-      <c r="E994" s="7"/>
-      <c r="F994" s="7"/>
-      <c r="G994" s="7"/>
-      <c r="H994" s="7"/>
-      <c r="I994" s="7"/>
-      <c r="J994" s="7"/>
-      <c r="K994" s="7"/>
-      <c r="L994" s="7"/>
-      <c r="M994" s="7"/>
-      <c r="N994" s="7"/>
-      <c r="O994" s="7"/>
-      <c r="P994" s="7"/>
-      <c r="Q994" s="7"/>
-      <c r="R994" s="7"/>
-      <c r="S994" s="7"/>
-      <c r="T994" s="7"/>
-      <c r="U994" s="7"/>
-      <c r="V994" s="7"/>
-      <c r="W994" s="7"/>
-      <c r="X994" s="7"/>
-      <c r="Y994" s="7"/>
-      <c r="Z994" s="7"/>
-    </row>
-    <row r="995">
-      <c r="A995" s="7"/>
-      <c r="B995" s="7"/>
-      <c r="C995" s="7"/>
-      <c r="D995" s="7"/>
-      <c r="E995" s="7"/>
-      <c r="F995" s="7"/>
-      <c r="G995" s="7"/>
-      <c r="H995" s="7"/>
-      <c r="I995" s="7"/>
-      <c r="J995" s="7"/>
-      <c r="K995" s="7"/>
-      <c r="L995" s="7"/>
-      <c r="M995" s="7"/>
-      <c r="N995" s="7"/>
-      <c r="O995" s="7"/>
-      <c r="P995" s="7"/>
-      <c r="Q995" s="7"/>
-      <c r="R995" s="7"/>
-      <c r="S995" s="7"/>
-      <c r="T995" s="7"/>
-      <c r="U995" s="7"/>
-      <c r="V995" s="7"/>
-      <c r="W995" s="7"/>
-      <c r="X995" s="7"/>
-      <c r="Y995" s="7"/>
-      <c r="Z995" s="7"/>
-    </row>
-    <row r="996">
-      <c r="A996" s="7"/>
-      <c r="B996" s="7"/>
-      <c r="C996" s="7"/>
-      <c r="D996" s="7"/>
-      <c r="E996" s="7"/>
-      <c r="F996" s="7"/>
-      <c r="G996" s="7"/>
-      <c r="H996" s="7"/>
-      <c r="I996" s="7"/>
-      <c r="J996" s="7"/>
-      <c r="K996" s="7"/>
-      <c r="L996" s="7"/>
-      <c r="M996" s="7"/>
-      <c r="N996" s="7"/>
-      <c r="O996" s="7"/>
-      <c r="P996" s="7"/>
-      <c r="Q996" s="7"/>
-      <c r="R996" s="7"/>
-      <c r="S996" s="7"/>
-      <c r="T996" s="7"/>
-      <c r="U996" s="7"/>
-      <c r="V996" s="7"/>
-      <c r="W996" s="7"/>
-      <c r="X996" s="7"/>
-      <c r="Y996" s="7"/>
-      <c r="Z996" s="7"/>
-    </row>
-    <row r="997">
-      <c r="A997" s="7"/>
-      <c r="B997" s="7"/>
-      <c r="C997" s="7"/>
-      <c r="D997" s="7"/>
-      <c r="E997" s="7"/>
-      <c r="F997" s="7"/>
-      <c r="G997" s="7"/>
-      <c r="H997" s="7"/>
-      <c r="I997" s="7"/>
-      <c r="J997" s="7"/>
-      <c r="K997" s="7"/>
-      <c r="L997" s="7"/>
-      <c r="M997" s="7"/>
-      <c r="N997" s="7"/>
-      <c r="O997" s="7"/>
-      <c r="P997" s="7"/>
-      <c r="Q997" s="7"/>
-      <c r="R997" s="7"/>
-      <c r="S997" s="7"/>
-      <c r="T997" s="7"/>
-      <c r="U997" s="7"/>
-      <c r="V997" s="7"/>
-      <c r="W997" s="7"/>
-      <c r="X997" s="7"/>
-      <c r="Y997" s="7"/>
-      <c r="Z997" s="7"/>
-    </row>
-    <row r="998">
-      <c r="A998" s="7"/>
-      <c r="B998" s="7"/>
-      <c r="C998" s="7"/>
-      <c r="D998" s="7"/>
-      <c r="E998" s="7"/>
-      <c r="F998" s="7"/>
-      <c r="G998" s="7"/>
-      <c r="H998" s="7"/>
-      <c r="I998" s="7"/>
-      <c r="J998" s="7"/>
-      <c r="K998" s="7"/>
-      <c r="L998" s="7"/>
-      <c r="M998" s="7"/>
-      <c r="N998" s="7"/>
-      <c r="O998" s="7"/>
-      <c r="P998" s="7"/>
-      <c r="Q998" s="7"/>
-      <c r="R998" s="7"/>
-      <c r="S998" s="7"/>
-      <c r="T998" s="7"/>
-      <c r="U998" s="7"/>
-      <c r="V998" s="7"/>
-      <c r="W998" s="7"/>
-      <c r="X998" s="7"/>
-      <c r="Y998" s="7"/>
-      <c r="Z998" s="7"/>
-    </row>
-    <row r="999">
-      <c r="A999" s="7"/>
-      <c r="B999" s="7"/>
-      <c r="C999" s="7"/>
-      <c r="D999" s="7"/>
-      <c r="E999" s="7"/>
-      <c r="F999" s="7"/>
-      <c r="G999" s="7"/>
-      <c r="H999" s="7"/>
-      <c r="I999" s="7"/>
-      <c r="J999" s="7"/>
-      <c r="K999" s="7"/>
-      <c r="L999" s="7"/>
-      <c r="M999" s="7"/>
-      <c r="N999" s="7"/>
-      <c r="O999" s="7"/>
-      <c r="P999" s="7"/>
-      <c r="Q999" s="7"/>
-      <c r="R999" s="7"/>
-      <c r="S999" s="7"/>
-      <c r="T999" s="7"/>
-      <c r="U999" s="7"/>
-      <c r="V999" s="7"/>
-      <c r="W999" s="7"/>
-      <c r="X999" s="7"/>
-      <c r="Y999" s="7"/>
-      <c r="Z999" s="7"/>
-    </row>
-    <row r="1000">
-      <c r="A1000" s="7"/>
-      <c r="B1000" s="7"/>
-      <c r="C1000" s="7"/>
-      <c r="D1000" s="7"/>
-      <c r="E1000" s="7"/>
-      <c r="F1000" s="7"/>
-      <c r="G1000" s="7"/>
-      <c r="H1000" s="7"/>
-      <c r="I1000" s="7"/>
-      <c r="J1000" s="7"/>
-      <c r="K1000" s="7"/>
-      <c r="L1000" s="7"/>
-      <c r="M1000" s="7"/>
-      <c r="N1000" s="7"/>
-      <c r="O1000" s="7"/>
-      <c r="P1000" s="7"/>
-      <c r="Q1000" s="7"/>
-      <c r="R1000" s="7"/>
-      <c r="S1000" s="7"/>
-      <c r="T1000" s="7"/>
-      <c r="U1000" s="7"/>
-      <c r="V1000" s="7"/>
-      <c r="W1000" s="7"/>
-      <c r="X1000" s="7"/>
-      <c r="Y1000" s="7"/>
-      <c r="Z1000" s="7"/>
-    </row>
   </sheetData>
-  <autoFilter ref="$C$1:$C$1000"/>
+  <autoFilter ref="$C$1:$C$992"/>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="D2"/>
     <hyperlink r:id="rId2" ref="D3"/>
@@ -29409,7 +30315,44 @@
     <hyperlink r:id="rId30" ref="D31"/>
     <hyperlink r:id="rId31" ref="D32"/>
     <hyperlink r:id="rId32" ref="D33"/>
+    <hyperlink r:id="rId33" ref="D34"/>
+    <hyperlink r:id="rId34" ref="D35"/>
+    <hyperlink r:id="rId35" ref="D36"/>
+    <hyperlink r:id="rId36" ref="D37"/>
+    <hyperlink r:id="rId37" ref="D39"/>
+    <hyperlink r:id="rId38" ref="D40"/>
+    <hyperlink r:id="rId39" ref="D41"/>
+    <hyperlink r:id="rId40" ref="D42"/>
+    <hyperlink r:id="rId41" ref="D43"/>
+    <hyperlink r:id="rId42" ref="D44"/>
+    <hyperlink r:id="rId43" ref="D45"/>
+    <hyperlink r:id="rId44" ref="D46"/>
+    <hyperlink r:id="rId45" ref="D47"/>
+    <hyperlink r:id="rId46" ref="D48"/>
+    <hyperlink r:id="rId47" ref="D49"/>
+    <hyperlink r:id="rId48" ref="D50"/>
+    <hyperlink r:id="rId49" ref="D51"/>
+    <hyperlink r:id="rId50" ref="D52"/>
+    <hyperlink r:id="rId51" ref="D53"/>
+    <hyperlink r:id="rId52" ref="D54"/>
+    <hyperlink r:id="rId53" ref="D55"/>
+    <hyperlink r:id="rId54" ref="D56"/>
+    <hyperlink r:id="rId55" ref="D57"/>
+    <hyperlink r:id="rId56" ref="D58"/>
+    <hyperlink r:id="rId57" ref="D59"/>
+    <hyperlink r:id="rId58" ref="D60"/>
+    <hyperlink r:id="rId59" ref="D61"/>
+    <hyperlink r:id="rId60" ref="D62"/>
+    <hyperlink r:id="rId61" ref="D63"/>
+    <hyperlink r:id="rId62" ref="D64"/>
+    <hyperlink r:id="rId63" ref="D65"/>
+    <hyperlink r:id="rId64" ref="D66"/>
+    <hyperlink r:id="rId65" ref="D67"/>
+    <hyperlink r:id="rId66" ref="D68"/>
+    <hyperlink r:id="rId67" ref="D69"/>
+    <hyperlink r:id="rId68" ref="D70"/>
+    <hyperlink r:id="rId69" ref="D71"/>
   </hyperlinks>
-  <drawing r:id="rId33"/>
+  <drawing r:id="rId70"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Insert data on QDrant
</commit_message>
<xml_diff>
--- a/data/Info RAG.xlsx
+++ b/data/Info RAG.xlsx
@@ -153,11 +153,11 @@
   <si>
     <t xml:space="preserve">PLANTA MEDICINAL: Alecrim
 INDICAÇÕES:
- Uso interno: Anti-inflamatório e distúrbios digestivos. Atua no tratamento de fadiga, dores de cabeça, enxaquecas, má circulação, problemas de concentração e memória, distúrbios respiratórios, gripe, febre, contusões, artrite, artrose, cistite, menstruação irregular, cólica menstrual, tensão pré-menstrual (TPM).
- Uso externo: Anti-inflamatório e possui ação cicatrizante.
+- Uso interno: Anti-inflamatório e distúrbios digestivos. Atua no tratamento de fadiga, dores de cabeça, enxaquecas, má circulação, problemas de concentração e memória, distúrbios respiratórios, gripe, febre, contusões, artrite, artrose, cistite, menstruação irregular, cólica menstrual, tensão pré-menstrual (TPM).
+- Uso externo: Anti-inflamatório e possui ação cicatrizante.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão - 1 colher de sobremesa (2 g) de folhas secas de alecrim para 1 xícara de chá (150 mL) de água. A infusão deve ser tomada, ainda morna, de 2 a 4 vezes ao dia.
- Uso externo: Infusão - 30 a 50 g da planta para 1 L de água. Utilizar morno. Realizar compressa ou banho.
+- Uso interno: Infusão - 1 colher de sobremesa (2 g) de folhas secas de alecrim para 1 xícara de chá (150 mL) de água. A infusão deve ser tomada, ainda morna, de 2 a 4 vezes ao dia.
+- Uso externo: Infusão - 30 a 50 g da planta para 1 L de água. Utilizar morno. Realizar compressa ou banho.
 CUIDADOS: Em doses elevadas pode causar irritação gastrointestinal. Evitar o consumo à noite, pois pode prejudicar o sono. É contraindicado em caso de gravidez, histórico de convulsões, gastroenterite
 </t>
   </si>
@@ -170,19 +170,19 @@
   <si>
     <t>PLANTA MEDICINAL: Babosa
 INDICAÇÕES:
- Uso externo: Cicatrizante, anti-inflamatório, analgésico, emoliente e antisséptico. Para lesões de pele secundárias a queimaduras térmicas ou químicas (primeiro e segundo graus) e físicas (radioterapia), dermatites (periostomia e outras), eczemas, psoríase, queda de cabelo por seborreia, acne vulgar, celulite e erisipela. Observa-se alívio da dor em queimaduras.
+- Uso externo: Cicatrizante, anti-inflamatório, analgésico, emoliente e antisséptico. Para lesões de pele secundárias a queimaduras térmicas ou químicas (primeiro e segundo graus) e físicas (radioterapia), dermatites (periostomia e outras), eczemas, psoríase, queda de cabelo por seborreia, acne vulgar, celulite e erisipela. Observa-se alívio da dor em queimaduras.
 POSOLOGIA E MODO DE PREPARO:
-Uso externo: 
+- Uso externo: 
 Cataplasma - Retire uma folha pela base. Cortar a outra extremidade e deixar em pé com a base para baixo por duas horas, para escoar o líquido amarelado e de odor forte. Lavar em água corrente, descascar sem deixar a parte verde no gel. Picar o gel e bater em liquidificador previamente higienizado por cerca de 40 segundos para manter a consistência do gel. Como a folha é formada por 95% de água, se bater muito a consistência ficará líquida. Deixar em repouso por 15 minutos para que a espuma que se forma diminua. Aplicá-lo diretamente sobre a lesão de 2 a 3 vezes ao dia. Cubra a lesão com gaze e mantenha ocluído até a próxima troca.
 Compressa - uma folha grande é aberta ao meio e colocada sobre uma porção de algodão ou gaze para captar a mucilagem, em seguida aplica-se sobre a pele. Aplicar na área afetada 1 a 3 vezes ao dia. Manter a lesão ocluída com a compressa.</t>
   </si>
   <si>
     <t>PLANTA MEDICINAL: Boldo
 INDICAÇÕES:
- Uso interno: Estimulante do fígado, da digestão e do apetite, atua na melhora
+- Uso interno: Estimulante do fígado, da digestão e do apetite, atua na melhora
 da azia.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: 
+- Uso interno: 
 Infusão - 1 a 3 colheres de chá (1 a 3 g) de folhas secas para 1 xicara de chá (150 mL) de água. Acima de 12 anos tomar 150 mL do infuso, logo após o preparo, 2 a 3 vezes ao dia.
 Maceração - amassar ou picar 1 a 2 folhas frescas para 1 xicara de chá (150 mL) de água fria e deixar repousar por alguns minutos, 2 a 3 vezes ao dia.
 CUIDADOS: Não deve ser utilizado por gestantes, lactantes, crianças e portadores de obstrução das vias biliares ou cálculos biliares (pedra na vesícula). Não usar no caso de tratamento com metronidazol ou dissulfiram, medicamentos depressores do sistema nervoso central (SNC) e anti-hipertensivos. Doses acima das recomendadas e utilizadas por um período maior do que o recomendado podem causar irritação gástrica.</t>
@@ -190,100 +190,100 @@
   <si>
     <t>PLANTA MEDICINAL: Calêndula
 INDICAÇÕES:
- Uso interno: Digestório e imunoestimulante.
- Uso externo: Cicatrizante e anti-inflamatório nas feridas. Em bochecho ou gargarejo, utilizar para gengivite e estomatites.
+- Uso interno: Digestório e imunoestimulante.
+- Uso externo: Cicatrizante e anti-inflamatório nas feridas. Em bochecho ou gargarejo, utilizar para gengivite e estomatites.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão - 1 a 2 colheres de chá (1 a 2 g) de inflorescências secas para 1 xícara de chá (150 mL) de água, 2 vezes ao dia.
- Uso externo: Infusão – 1 a 2 colheres de chá (1 a 2 g) de inflorescências secas para 1 xícara de chá (150 mL) de água. Utilizar em banho, compressa na área afetada ou sob a forma de bochecho ou gargarejo, 3 vezes ao dia.
+- Uso interno: Infusão - 1 a 2 colheres de chá (1 a 2 g) de inflorescências secas para 1 xícara de chá (150 mL) de água, 2 vezes ao dia.
+- Uso externo: Infusão – 1 a 2 colheres de chá (1 a 2 g) de inflorescências secas para 1 xícara de chá (150 mL) de água. Utilizar em banho, compressa na área afetada ou sob a forma de bochecho ou gargarejo, 3 vezes ao dia.
 CUIDADOS: Contraindicado o uso interno durante a gravidez e lactação.</t>
   </si>
   <si>
     <t>PLANTA MEDICINAL: Capim-limão
 INDICAÇÕES:
- Uso interno: Antiespasmódico (do sistema digestório), problemas respiratórios (expectorante e descongestionante) e sedativo leve.
+- Uso interno: Antiespasmódico (do sistema digestório), problemas respiratórios (expectorante e descongestionante) e sedativo leve.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão – 1 a 3 colheres de chá (1 a 3 g) de planta seca para 1 xícara de chá (150 mL) de água. Acima de 12 anos: tomar 150 mL do infuso, após amornar, duas a três vezes ao dia. Para problemas respiratórios utilizar o chá da planta fresca na mesma quantidade.
+- Uso interno: Infusão – 1 a 3 colheres de chá (1 a 3 g) de planta seca para 1 xícara de chá (150 mL) de água. Acima de 12 anos: tomar 150 mL do infuso, após amornar, duas a três vezes ao dia. Para problemas respiratórios utilizar o chá da planta fresca na mesma quantidade.
 CUIDADOS: Pode potencializar o efeito de medicamentos sedativos. Contraindicado o uso interno durante a gravidez</t>
   </si>
   <si>
     <t>PLANTA MEDICINAL: Carqueja
 INDICAÇÕES:
- Uso interno: Auxilia no tratamento das doenças digestivas em geral e dos distúrbios hepáticos. Também possui ação diurética e depurativa, antiinflamatória para dores articulares, sendo indicado para casos de gota.
- Uso externo: Dor de garganta.
+- Uso interno: Auxilia no tratamento das doenças digestivas em geral e dos distúrbios hepáticos. Também possui ação diurética e depurativa, antiinflamatória para dores articulares, sendo indicado para casos de gota.
+- Uso externo: Dor de garganta.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão - 2,5 g de planta seca para uma xícara de chá (150 mL) de água. Acima de 12 anos tomar 150 mL do infuso, logo após o preparo, 2 a 3 vezes ao dia.
- Uso externo: Infusão - 2,5 g de planta seca para uma xícara de chá (150 mL) de água. Utilizar em forma de gargarejo, 2 a 3 vezes ao dia.
+- Uso interno: Infusão - 2,5 g de planta seca para uma xícara de chá (150 mL) de água. Acima de 12 anos tomar 150 mL do infuso, logo após o preparo, 2 a 3 vezes ao dia.
+- Uso externo: Infusão - 2,5 g de planta seca para uma xícara de chá (150 mL) de água. Utilizar em forma de gargarejo, 2 a 3 vezes ao dia.
 CUIDADOS: Não utilizar em gestantes e lactantes. Em dose excessiva pode provocar contrações uterinas. O uso pode causar hipotensão. Evitar o uso concomitante com medicamentos para hipertensão e diabetes.</t>
   </si>
   <si>
     <t>PLANTA MEDICINAL: Cúrcuma
 INDICAÇÕES:
- Uso interno: Ação digestória, antimicrobiana e anti-inflamatória.
+- Uso interno: Ação digestória, antimicrobiana e anti-inflamatória.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão - 1,5 g de rizoma picado para 1 xícara de chá (150 mL), 2 vezes ao dia.
+- Uso interno: Infusão - 1,5 g de rizoma picado para 1 xícara de chá (150 mL), 2 vezes ao dia.
 CUIDADOS: O uso é contraindicado para pessoas com cálculos biliares, obstrução dos ductos biliares e úlcera gastroduodenal. Não utilizar em caso de tratamento com anticoagulantes.</t>
   </si>
   <si>
     <t xml:space="preserve">PLANTA MEDICINAL:  Erva-baleeira
 INDICAÇÕES:
- Uso interno e externo: Inflamações e dores em articulações, tendões e músculos; no reumatismo, artrites e nas contusões.
- Uso externo: Auxiliar na cicatrização de úlceras e feridas.
+- Uso interno e externo: Inflamações e dores em articulações, tendões e músculos; no reumatismo, artrites e nas contusões.
+- Uso externo: Auxiliar na cicatrização de úlceras e feridas.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão - 1,5 g de folhas secas para uma xícara de chá (150 mL) de água. Acima de 12 anos tomar 2 a 3 vezes ao dia.
- Uso externo: Infusão - 1,5 g de folhas secas para uma xícara de chá (150 mL) de água. Realizar compressas, 3 vezes ao dia.
+- Uso interno: Infusão - 1,5 g de folhas secas para uma xícara de chá (150 mL) de água. Acima de 12 anos tomar 2 a 3 vezes ao dia.
+- Uso externo: Infusão - 1,5 g de folhas secas para uma xícara de chá (150 mL) de água. Realizar compressas, 3 vezes ao dia.
 Cataplasma - com as folhas frescas, 3 vezes ao dia.
 CUIDADOS: Nas quantidades corretas é uma planta bastante segura e de baixíssima toxicidade. Deve ser evitada por gestantes e lactantes. </t>
   </si>
   <si>
     <t>PLANTA MEDICINAL:  Erva cidreira brasileira
 INDICAÇÕES:
- Uso interno: Antiespasmódica (cólicas uterinas e intestinais), analgésica, antidispéptico, ansiolítico e sedativo leve (calmante e insônia), hipotensora leve, antigripal, expectorante e auxiliar em dor de cabeça. Auxilia em TPM, síndrome do climatério e síndrome do intestino irritável e diarreias.
+- Uso interno: Antiespasmódica (cólicas uterinas e intestinais), analgésica, antidispéptico, ansiolítico e sedativo leve (calmante e insônia), hipotensora leve, antigripal, expectorante e auxiliar em dor de cabeça. Auxilia em TPM, síndrome do climatério e síndrome do intestino irritável e diarreias.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão - 1 a 3 colheres de chá (1 a 3 g) de partes aéreas secas para 1 xícara de chá (150 mL) de água. De 3 a 7 anos tomar 35 mL do infuso 3 a 4 vezes ao dia. De 7 a 12 anos 75 mL do infuso 2 a 3 vezes dia. Acima de 12 anos tomar 150 mL do infuso 2 a 4 vezes dia. Acima de 70 anos tomar 75 mL do infuso 2 a 3 vezes dia.
+- Uso interno: Infusão - 1 a 3 colheres de chá (1 a 3 g) de partes aéreas secas para 1 xícara de chá (150 mL) de água. De 3 a 7 anos tomar 35 mL do infuso 3 a 4 vezes ao dia. De 7 a 12 anos 75 mL do infuso 2 a 3 vezes dia. Acima de 12 anos tomar 150 mL do infuso 2 a 4 vezes dia. Acima de 70 anos tomar 75 mL do infuso 2 a 3 vezes dia.
 CUIDADOS: evitar o uso durante a gravidez, lactação em caso de hipotensão. Pode aumentar a toxicidade de paracetamol se usado concomitantemente. Doses acimas da recomendada podem causar irritação gástrica, bradicardia e hipotensão.</t>
   </si>
   <si>
     <t>PLANTA MEDICINAL: Espinheira-santa
 INDICAÇÕES:
- Uso interno: Gastrites, úlceras gástrica e duodenal, atividade anti-inflamatória. Apresenta efeito adstringente, aumenta a barreira de mucosa no estômago, diminui a secreção de ácido clorídrico. Efetiva contra Helicobacter pylori. Cicatrizante, levemente diurética e laxativa. Antisséptica, reduzindo a formação de gases (carminativa).
+- Uso interno: Gastrites, úlceras gástrica e duodenal, atividade anti-inflamatória. Apresenta efeito adstringente, aumenta a barreira de mucosa no estômago, diminui a secreção de ácido clorídrico. Efetiva contra Helicobacter pylori. Cicatrizante, levemente diurética e laxativa. Antisséptica, reduzindo a formação de gases (carminativa).
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão – 1 colher de sopa (3 g) das folhas secas para uma xícara de chá (150 mL) de água, 3 a 4 vezes ao dia (1 hora após as refeições e 1 hora antes de deitar-se). Tempo de tratamento proposto em torno de 28 dias.
+- Uso interno: Infusão – 1 colher de sopa (3 g) das folhas secas para uma xícara de chá (150 mL) de água, 3 a 4 vezes ao dia (1 hora após as refeições e 1 hora antes de deitar-se). Tempo de tratamento proposto em torno de 28 dias.
 CUIDADOS: Contraindicado o uso durante a gravidez, por lactantes (reduz a secreção láctea) e por crianças menores de 6 anos. Pode haver interação medicamentosa com antibióticos e barbitúricos. Em alguns casos foram observados: boca seca e gosto estranho na boca.</t>
   </si>
   <si>
     <t>PLANTA MEDICINAL: Funcho
 INDICAÇÕES:
- Uso interno: Frutos (sementes): ação antiespasmódica (cólicas digestivas e menstruais), hepatoprotetora, carminativa (flatulência), antimicrobiana e expectorante (tosse e bronquite). Estimula o apetite, facilita a lactação (estimula o leite materno), descongestionante das vias aéreas superiores. Folhas: digestiva, sedativa, cicatrizante e antisséptica.
+- Uso interno: Frutos (sementes): ação antiespasmódica (cólicas digestivas e menstruais), hepatoprotetora, carminativa (flatulência), antimicrobiana e expectorante (tosse e bronquite). Estimula o apetite, facilita a lactação (estimula o leite materno), descongestionante das vias aéreas superiores. Folhas: digestiva, sedativa, cicatrizante e antisséptica.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão - 1 colher de sopa (3 g) de frutos secos (sementes) em uma xícara de chá (150 mL) de água. Tomar 2 a 3 vezes ao dia.
+- Uso interno: Infusão - 1 colher de sopa (3 g) de frutos secos (sementes) em uma xícara de chá (150 mL) de água. Tomar 2 a 3 vezes ao dia.
 CUIDADOS:  aumenta o fluxo menstrual. Evitar nos casos de hiperandrogenismo e hiperestrogenismo e uso por gestantes.</t>
   </si>
   <si>
     <t>PLANTA MEDICINAL: Gengibre
 INDICAÇÕES:
- Uso interno: Carminativa (combate gases intestinais), antiemética, digestória, combate arterioesclerose, ação antioxidante, antisséptico e anti-inflamatório para problemas respiratórios (expectorante e dor de garganta) e casos de cinetose (enjoo por movimento em carros, aviões e barcos).
- Uso externo: Inflamações de boca e garganta.
+- Uso interno: Carminativa (combate gases intestinais), antiemética, digestória, combate arterioesclerose, ação antioxidante, antisséptico e anti-inflamatório para problemas respiratórios (expectorante e dor de garganta) e casos de cinetose (enjoo por movimento em carros, aviões e barcos).
+- Uso externo: Inflamações de boca e garganta.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão ou decocção - 0,5 g a 1,0 g do rizoma (picado para decocção ou ralado para infusão) para 1 xícara de chá (150 mL) de água. Após o procedimento, tanto na infusão, quanto na decocção, deixar o recipiente tampado por no mínimo 10 minutos. Tomar 2 a 4 vezes ao dia.
- Uso externo: Infusão ou decocção - 0,5 a 1,0 g do rizoma (picado para decocção ou ralado para infusão) para 1 xícara de chá (150 mL) de água. Após o procedimento, tanto na infusão, quanto na decocção, deixar o recipiente tampado por no mínimo 10 minutos. Realizar bochecho ou gargarejo 2 a 4 vezes ao dia.
+- Uso interno: Infusão ou decocção - 0,5 g a 1,0 g do rizoma (picado para decocção ou ralado para infusão) para 1 xícara de chá (150 mL) de água. Após o procedimento, tanto na infusão, quanto na decocção, deixar o recipiente tampado por no mínimo 10 minutos. Tomar 2 a 4 vezes ao dia.
+- Uso externo: Infusão ou decocção - 0,5 a 1,0 g do rizoma (picado para decocção ou ralado para infusão) para 1 xícara de chá (150 mL) de água. Após o procedimento, tanto na infusão, quanto na decocção, deixar o recipiente tampado por no mínimo 10 minutos. Realizar bochecho ou gargarejo 2 a 4 vezes ao dia.
 CUIDADOS: Não utilizar em gravidez e lactação em doses maiores que 1 colher de café por dia (0,5 g). Não utilizar para crianças menores de 6 anos. Contraindicado seu uso para pessoas com úlcera péptica, colite, doença hepática, cálculo biliar, hipertensão arterial ou concomitante com anticoagulantes.</t>
   </si>
   <si>
     <t>PLANTA MEDICINAL: Goiabeira
 INDICAÇÕES:
- Uso interno: Folhas, cascas e frutos verdes possuem ação antidiarreica e antioxidante; frutos maduros possuem ação espasmolítica (diminuem cólicas intestinais) e digestória.
- Uso externo: Folhas, cascas e frutos verdes possuem atividade antimicrobiana e antiinflamatória para feridas e gargarejos.
+- Uso interno: Folhas, cascas e frutos verdes possuem ação antidiarreica e antioxidante; frutos maduros possuem ação espasmolítica (diminuem cólicas intestinais) e digestória.
+- Uso externo: Folhas, cascas e frutos verdes possuem atividade antimicrobiana e antiinflamatória para feridas e gargarejos.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão - 3 a 4 brotos (cada um possui em torno de 2-3 folhas jovens) em 1 xícara de chá (150 mL) de água, tampar e após amornar tomar 50 mL para casos de diarreia não infecciosa. Observar. Se necessário, administrar mais 50 mL após 4 horas.
- Uso externo: Decocção - 10 folhas fervidas para 1 litro de água, por 2 ou 3 minutos. Para feridas: esfriar e deixar em contato com as feridas (banho ou compressa) por 20 minutos (mínimo), utilizar 1 a 2 vezes ao dia. Para gargarejo: utilizar 2 a 3 vezes ao dia.
+- Uso interno: Infusão - 3 a 4 brotos (cada um possui em torno de 2-3 folhas jovens) em 1 xícara de chá (150 mL) de água, tampar e após amornar tomar 50 mL para casos de diarreia não infecciosa. Observar. Se necessário, administrar mais 50 mL após 4 horas.
+- Uso externo: Decocção - 10 folhas fervidas para 1 litro de água, por 2 ou 3 minutos. Para feridas: esfriar e deixar em contato com as feridas (banho ou compressa) por 20 minutos (mínimo), utilizar 1 a 2 vezes ao dia. Para gargarejo: utilizar 2 a 3 vezes ao dia.
 CUIDADOS: O uso interno é contraindicado para grávidas, lactantes, crianças de 3 anos e não deve ser utilizado por mais de 30 dias ou em caso de diarreia infecciosa. O uso externo não deve ser utilizado por grávidas e lactantes com lesões extensas e graves.</t>
   </si>
   <si>
     <t>PLANTA MEDICINAL: Guaco
 INDICAÇÕES:
- Uso interno: Expectorante, broncodilatador.
+- Uso interno: Expectorante, broncodilatador.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: 
+- Uso interno: 
 Infusão - 1 colher de sopa (3 g) de folhas secas para 1 xícara de chá (150 mL) de água. Acima de 12 anos: 2 vezes ao dia, logo após o preparo. Xarope caseiro - 20 folhas frescas picadas para 1 xícara de chá (150 mL) de água e 1 e ½ xícara de chá (255 g) de açúcar. Cozinhar em calor brando as folhas em água, sempre tampado, por 5 minutos, até perceber o odor adocicado de cumarina. Coar e acrescentar o açúcar até dissolver, se necessário, aquecer brandamente (60 a 80° C). Acondicionar em recipiente higienizado, de preferência em vidro âmbar. Armazenar em geladeira ou em local fresco e ao abrigo da luz. Esta preparação não pode ser usada por mais de 7 dias e deve-se verificar frequentemente se o xarope não fermentou (azedou). Crianças de 3 a 6 anos: tomar 1 colher de chá (5 mL), 2 vezes ao dia. Crianças de 7 a 12 anos: tomar uma colher de sobremesa (10 mL), 3 vezes ao dia. Acima de 12 anos: tomar uma colher de sopa (15 mL), 3 vezes ao dia. Agitar antes de usar.
 Atenção: contraindicado a pacientes portadores de Diabetes mellitus, gestantes, lactantes e crianças menores de dois anos e em caso de tratamento com anticoagulantes.
 CUIDADOS: Não utilizar em caso de tratamento com anticoagulante. A utilização pode interferir na coagulação sanguínea. Doses acima das recomendadas podem provocar vômitos e diarreia.</t>
@@ -291,59 +291,59 @@
   <si>
     <t xml:space="preserve">PLANTA MEDICINAL: Hortelã
 INDICAÇÕES:
- Uso interno: auxiliar da digestão, tratamento de parasitoses intestinais e diarreias causadas por ameba e giardíase (Giardia lamblia).
- Uso externo: no tratamento de tricomoníase (Trichomonas vaginalis )
+- Uso interno: auxiliar da digestão, tratamento de parasitoses intestinais e diarreias causadas por ameba e giardíase (Giardia lamblia).
+- Uso externo: no tratamento de tricomoníase (Trichomonas vaginalis )
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: 
+- Uso interno: 
 Infusão - 1 colher de sopa (3 g) de folhas frescas ou 1 colher de chá (1 g) de folhas secas para 1 xícara de chá (150 mL) de água. O chá deve ser tomado de 2 a 4 vezes ao dia.
 Pó vegetal - para tratamento de parasitoses intestinais e diarreias causadas por ameba e giardíase (Giardia lamblia). Crianças de 5 a 13 anos: ¼ de uma colher de café (100-150 mg) do pó, 3 vezes ao dia durante 5 dias. Acima de 13 anos: ½ colher de café (200-300 mg) do pó, 3 vezes ao dia durante 5 dias. Em ambos os casos, o tratamento deve ser repetido após 10 dias.
- Uso externo: Infusão - 1 colher de sopa (3 g) de folhas frescas ou 1 colher de chá (1 g) de folhas secas para 1 xícara de chá (150 mL) de água. Fazer banho de assento diariamente durante 1 a 2 semanas. Deve ser associado com o uso interno.
+- Uso externo: Infusão - 1 colher de sopa (3 g) de folhas frescas ou 1 colher de chá (1 g) de folhas secas para 1 xícara de chá (150 mL) de água. Fazer banho de assento diariamente durante 1 a 2 semanas. Deve ser associado com o uso interno.
 </t>
   </si>
   <si>
     <t>PLANTA MEDICINAL: Malvarisco
 INDICAÇÕES:
- Uso interno: contra gripe, problemas respiratórios, inflamações de boca e garganta.
+- Uso interno: contra gripe, problemas respiratórios, inflamações de boca e garganta.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Xarope caseiro: 30 folhas frescas de malvarisco lavadas e picadas e 1 xicara de chá (170 g) de açúcar. Em uma panela de vidro, inox ou esmaltada, intercalar com camadas de açúcar e folhas, começando com o açúcar. Observação: não vai água! Colocar em banho-maria por 40 minutos, tampado. Coar e tomar. De 2 a 6 anos, tomar 1 colher de chá (5 mL) do xarope 3 vezes ao dia. De 7 a 12 anos, tomar 1 colher de sobremesa (10 mL) do xarope 3 vezes ao dia. Acima de 12 anos, tomar 1 colher de sopa (15 mL) do xarope 3 vezes ao dia.
+- Uso interno: Xarope caseiro: 30 folhas frescas de malvarisco lavadas e picadas e 1 xicara de chá (170 g) de açúcar. Em uma panela de vidro, inox ou esmaltada, intercalar com camadas de açúcar e folhas, começando com o açúcar. Observação: não vai água! Colocar em banho-maria por 40 minutos, tampado. Coar e tomar. De 2 a 6 anos, tomar 1 colher de chá (5 mL) do xarope 3 vezes ao dia. De 7 a 12 anos, tomar 1 colher de sobremesa (10 mL) do xarope 3 vezes ao dia. Acima de 12 anos, tomar 1 colher de sopa (15 mL) do xarope 3 vezes ao dia.
 CUIDADOS: Não há relatos de contraindicações.</t>
   </si>
   <si>
     <t>PLANTA MEDICINAL: Melissa
 INDICAÇÕES:
- Uso interno: Antiespasmódico, digestivo, ansiolítico e sedativo leve.
+- Uso interno: Antiespasmódico, digestivo, ansiolítico e sedativo leve.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão – 1 colher de sopa (1 a 4 g) das partes aéreas secas para 1 xícara de chá (150 mL) de água. Acima de 12 anos: tomar 2 a 3 vezes ao dia.
+- Uso interno: Infusão – 1 colher de sopa (1 a 4 g) das partes aéreas secas para 1 xícara de chá (150 mL) de água. Acima de 12 anos: tomar 2 a 3 vezes ao dia.
 CUIDADOS:  Não deve ser utilizado nos casos de hipotireoidismo e por mulheres grávidas e lactantes; utilizar cuidadosamente em pessoas com hipotensão arterial.</t>
   </si>
   <si>
     <t>PLANTA MEDICINAL: Pitangueira
 INDICAÇÕES:
- Uso interno: antioxidante, diurética, digestiva, antidiarreica.
- Uso externo: atividade antimicrobiana para feridas e gargarejos.
+- Uso interno: antioxidante, diurética, digestiva, antidiarreica.
+- Uso externo: atividade antimicrobiana para feridas e gargarejos.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão - 10 g de folhas secas para 1 litro de água, tomar 2 a 3 xícaras de chá (150 mL) ao dia, após refeições.
- Uso externo: Decocção - 10 folhas para 1 litro de água. Para feridas: esfriar e deixar em contato com as feridas (banho ou compressa) por 20 minutos (mínimo), utilizar 1 a 2 vezes ao dia. Para gargarejo: utilizar 2 a 3 vezes ao dia.
+- Uso interno: Infusão - 10 g de folhas secas para 1 litro de água, tomar 2 a 3 xícaras de chá (150 mL) ao dia, após refeições.
+- Uso externo: Decocção - 10 folhas para 1 litro de água. Para feridas: esfriar e deixar em contato com as feridas (banho ou compressa) por 20 minutos (mínimo), utilizar 1 a 2 vezes ao dia. Para gargarejo: utilizar 2 a 3 vezes ao dia.
 CUIDADOS:  O uso interno é contraindicado para grávidas, lactantes, crianças de 3 anos e não deve ser utilizado por mais de 30 dias. O uso externo não deve ser utilizado por grávidas e lactantes com lesões extensas e graves.</t>
   </si>
   <si>
     <t>PLANTA MEDICINAL: Sálvia
 INDICAÇÕES:
- Uso interno: Antisséptica, infecções das vias respiratórias, tosse, rouquidão e estomatite, faringite e aftas. Dispepsias, anti-inflamatória, antioxidante e estrogênica, indicada na síndrome do climatério, irregularidades menstruais e supressão da lactação. Estimula o apetite e estudos comprovam melhorar a memória em idosos.
- Uso externo: Antisséptica, infecções das vias respiratórias, tosse, rouquidão e estomatite, faringite e aftas. Cicatrizante, anti-inflamatória e diminui a transpiração (indicada em sudorese de extremidades e enfermidades que causam sudorese) e salivação excessiva.
+- Uso interno: Antisséptica, infecções das vias respiratórias, tosse, rouquidão e estomatite, faringite e aftas. Dispepsias, anti-inflamatória, antioxidante e estrogênica, indicada na síndrome do climatério, irregularidades menstruais e supressão da lactação. Estimula o apetite e estudos comprovam melhorar a memória em idosos.
+- Uso externo: Antisséptica, infecções das vias respiratórias, tosse, rouquidão e estomatite, faringite e aftas. Cicatrizante, anti-inflamatória e diminui a transpiração (indicada em sudorese de extremidades e enfermidades que causam sudorese) e salivação excessiva.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão -1 colher de sopa (3 g) de folhas para 1 xícara de chá (150 mL) de água. Acima de 12 anos: tomar 2 a 3 vezes ao dia, após as refeições.
- Uso externo: Infusão – 1 colher de sopa (3 g) de folhas para 1 xícara de chá (150 mL) de água, após higienização aplicar a compressa no local afetado ou realizar bochecho, 3 vezes ao dia.
+- Uso interno: Infusão -1 colher de sopa (3 g) de folhas para 1 xícara de chá (150 mL) de água. Acima de 12 anos: tomar 2 a 3 vezes ao dia, após as refeições.
+- Uso externo: Infusão – 1 colher de sopa (3 g) de folhas para 1 xícara de chá (150 mL) de água, após higienização aplicar a compressa no local afetado ou realizar bochecho, 3 vezes ao dia.
 CUIDADOS: Segura em doses terapêuticas. Em doses acima da recomendada pode causar convulsões pela presença de tujona e cânfora, pode potencializar efeitos sedativos (barbitúricos e benzodiazepínicos) e interferir na atividade se associada a hipoglicemiantes e anticonvulsivantes. Evitar o uso na gravidez, lactação, insuficiência renal, epilepsia e tumores estrógeno–dependentes. Pode causar irritação tópica em pacientes sensíveis.</t>
   </si>
   <si>
     <t>PLANTA MEDICINAL: Tanchagem
 INDICAÇÕES:
- Uso interno: cicatrizante, ajuda a combater problemas gastrointestinais, expectorante para infecções de vias respiratórias e protetor de mucosa.
- Uso externo: anti-inflamatório e antisséptico da cavidade oral, auxilia no tratamento da dor de garganta e aftas e pode ser usado para banho de assento. As folhas na forma de cataplasma podem ser aplicadas sobre picada de insetos, feridas e queimaduras.
+- Uso interno: cicatrizante, ajuda a combater problemas gastrointestinais, expectorante para infecções de vias respiratórias e protetor de mucosa.
+- Uso externo: anti-inflamatório e antisséptico da cavidade oral, auxilia no tratamento da dor de garganta e aftas e pode ser usado para banho de assento. As folhas na forma de cataplasma podem ser aplicadas sobre picada de insetos, feridas e queimaduras.
 POSOLOGIA E MODO DE PREPARO:
- Uso interno: Infusão - 2 colheres de sopa (6 g) de folhas secas para 1 xícara de chá (150 mL) de água. Tampar e esperar pelo menos 15 minutos. Para infecções bucofaríngeas: tomar a cada 6 horas. Para problemas gastrointestinais: tomar a cada 8 horas
- Uso externo: 
+- Uso interno: Infusão - 2 colheres de sopa (6 g) de folhas secas para 1 xícara de chá (150 mL) de água. Tampar e esperar pelo menos 15 minutos. Para infecções bucofaríngeas: tomar a cada 6 horas. Para problemas gastrointestinais: tomar a cada 8 horas
+- Uso externo: 
 Cataplasma - folhas frescas são amassadas ou trituradas vigorosamente e aplicadas diretamente sobre a lesão, 3 vezes ao dia.
 Infusão: 2 a 3 colheres de sopa de folhas (6 g a 9 g) para 1 xícara de chá (150 mL) de água, após higienização aplicar a compressa no local afetado ou realizar bochecho, 3 vezes ao dia.
 CUIDADOS: Seu uso é contraindicado para gestantes e lactantes, pacientes com obstrução intestinal e pacientes com hipotensão arterial. Não engolir o produto após o bochecho e gargarejo.</t>
@@ -653,7 +653,7 @@
 CUIDADOS: Para maximizar os benefícios nutricionais, consulte um nutricionista para adaptar essas recomendações às suas necessidades específicas.</t>
   </si>
   <si>
-    <t>Alimentaç±ao saudável</t>
+    <t>Alimentação saudável</t>
   </si>
   <si>
     <t>https://www.posuscs.com.br/melhores-alimentos-para-ajudar-na-cicatrizacao-no-pos-operatorio/noticia/3099</t>

</xml_diff>